<commit_message>
fixed mistake in test record
</commit_message>
<xml_diff>
--- a/matlab/Test Matrix.xlsx
+++ b/matlab/Test Matrix.xlsx
@@ -925,6 +925,14 @@
     <xf numFmtId="167" fontId="0" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="167" fontId="0" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="167" fontId="0" fillId="7" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="7" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="7" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="7" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -955,14 +963,6 @@
     <xf numFmtId="2" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="7" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="0" fillId="7" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="0" fillId="7" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1550,11 +1550,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="86352640"/>
-        <c:axId val="86354944"/>
+        <c:axId val="86970368"/>
+        <c:axId val="86971904"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="86352640"/>
+        <c:axId val="86970368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="34"/>
@@ -1563,12 +1563,12 @@
         <c:axPos val="b"/>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="86354944"/>
+        <c:crossAx val="86971904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="86354944"/>
+        <c:axId val="86971904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -1578,7 +1578,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00000" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="86352640"/>
+        <c:crossAx val="86970368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1591,7 +1591,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1667,23 +1667,23 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="111013248"/>
-        <c:axId val="111031424"/>
+        <c:axId val="87346176"/>
+        <c:axId val="87364352"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="111013248"/>
+        <c:axId val="87346176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="0.0" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="111031424"/>
+        <c:crossAx val="87364352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="111031424"/>
+        <c:axId val="87364352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1691,20 +1691,19 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="111013248"/>
+        <c:crossAx val="87346176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000111" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000111" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000122" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000122" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1780,23 +1779,23 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="111063424"/>
-        <c:axId val="111064960"/>
+        <c:axId val="87388160"/>
+        <c:axId val="87389696"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="111063424"/>
+        <c:axId val="87388160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="0.0" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="111064960"/>
+        <c:crossAx val="87389696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="111064960"/>
+        <c:axId val="87389696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1804,20 +1803,19 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="111063424"/>
+        <c:crossAx val="87388160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000111" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000111" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000122" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000122" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1896,23 +1894,23 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="92505216"/>
-        <c:axId val="92513024"/>
+        <c:axId val="86992000"/>
+        <c:axId val="86993536"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="92505216"/>
+        <c:axId val="86992000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="0.0" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="92513024"/>
+        <c:crossAx val="86993536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="92513024"/>
+        <c:axId val="86993536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1920,20 +1918,19 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="92505216"/>
+        <c:crossAx val="86992000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000111" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000111" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000122" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000122" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2012,23 +2009,23 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="110876544"/>
-        <c:axId val="110878080"/>
+        <c:axId val="87029632"/>
+        <c:axId val="87031168"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="110876544"/>
+        <c:axId val="87029632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="0.0" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="110878080"/>
+        <c:crossAx val="87031168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="110878080"/>
+        <c:axId val="87031168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2036,20 +2033,19 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="110876544"/>
+        <c:crossAx val="87029632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000111" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000111" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000122" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000122" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2128,23 +2124,23 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="110787200"/>
-        <c:axId val="110788992"/>
+        <c:axId val="87181952"/>
+        <c:axId val="87204224"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="110787200"/>
+        <c:axId val="87181952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="0.0" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="110788992"/>
+        <c:crossAx val="87204224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="110788992"/>
+        <c:axId val="87204224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2152,20 +2148,19 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="110787200"/>
+        <c:crossAx val="87181952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000111" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000111" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000122" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000122" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2244,23 +2239,23 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="110808448"/>
-        <c:axId val="109646976"/>
+        <c:axId val="87215488"/>
+        <c:axId val="87221376"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="110808448"/>
+        <c:axId val="87215488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="0.0" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="109646976"/>
+        <c:crossAx val="87221376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="109646976"/>
+        <c:axId val="87221376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2268,20 +2263,19 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="110808448"/>
+        <c:crossAx val="87215488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000111" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000111" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000122" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000122" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2357,23 +2351,23 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="109674880"/>
-        <c:axId val="109676416"/>
+        <c:axId val="87249280"/>
+        <c:axId val="87250816"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="109674880"/>
+        <c:axId val="87249280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="0.0" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="109676416"/>
+        <c:crossAx val="87250816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="109676416"/>
+        <c:axId val="87250816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2381,20 +2375,19 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="109674880"/>
+        <c:crossAx val="87249280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000111" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000111" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000122" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000122" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2473,23 +2466,23 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="109696128"/>
-        <c:axId val="109697664"/>
+        <c:axId val="87274624"/>
+        <c:axId val="87276160"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="109696128"/>
+        <c:axId val="87274624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="0.0" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="109697664"/>
+        <c:crossAx val="87276160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="109697664"/>
+        <c:axId val="87276160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2497,20 +2490,19 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="109696128"/>
+        <c:crossAx val="87274624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000111" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000111" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000122" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000122" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2589,23 +2581,23 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="110966656"/>
-        <c:axId val="110968192"/>
+        <c:axId val="87299584"/>
+        <c:axId val="87301120"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="110966656"/>
+        <c:axId val="87299584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="0.0" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="110968192"/>
+        <c:crossAx val="87301120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="110968192"/>
+        <c:axId val="87301120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2613,20 +2605,19 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="110966656"/>
+        <c:crossAx val="87299584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000111" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000111" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000122" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000122" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2705,23 +2696,23 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="110996096"/>
-        <c:axId val="110997888"/>
+        <c:axId val="87324928"/>
+        <c:axId val="87339008"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="110996096"/>
+        <c:axId val="87324928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="0.0" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="110997888"/>
+        <c:crossAx val="87339008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="110997888"/>
+        <c:axId val="87339008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2729,20 +2720,19 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="110996096"/>
+        <c:crossAx val="87324928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000111" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000111" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000122" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000122" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3736,8 +3726,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AE73"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AF17" sqref="AF17"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H68" sqref="H68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3768,12 +3758,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:31" ht="15.75" thickBot="1">
-      <c r="H1" s="141"/>
-      <c r="I1" s="141"/>
-      <c r="M1" s="140" t="s">
+      <c r="H1" s="147"/>
+      <c r="I1" s="147"/>
+      <c r="M1" s="146" t="s">
         <v>30</v>
       </c>
-      <c r="N1" s="140"/>
+      <c r="N1" s="146"/>
       <c r="O1" s="38"/>
       <c r="P1" s="38"/>
       <c r="Q1" s="123"/>
@@ -3846,13 +3836,13 @@
       <c r="T2" s="134" t="s">
         <v>66</v>
       </c>
-      <c r="U2" s="149" t="s">
+      <c r="U2" s="139" t="s">
         <v>58</v>
       </c>
-      <c r="V2" s="144" t="s">
+      <c r="V2" s="150" t="s">
         <v>42</v>
       </c>
-      <c r="W2" s="144" t="s">
+      <c r="W2" s="150" t="s">
         <v>52</v>
       </c>
       <c r="X2" s="52" t="s">
@@ -3933,8 +3923,8 @@
       <c r="U3" s="30" t="s">
         <v>59</v>
       </c>
-      <c r="V3" s="145"/>
-      <c r="W3" s="145"/>
+      <c r="V3" s="151"/>
+      <c r="W3" s="151"/>
       <c r="X3" s="56" t="s">
         <v>47</v>
       </c>
@@ -4006,10 +3996,10 @@
         <v>12.320168196721314</v>
       </c>
       <c r="S4" s="136">
-        <f>R4/H4</f>
+        <f t="shared" ref="S4:S41" si="0">R4/H4</f>
         <v>0.80947228624975776</v>
       </c>
-      <c r="T4" s="150">
+      <c r="T4" s="140">
         <f>(H4-R4)/P4</f>
         <v>0.84991961606339728</v>
       </c>
@@ -4017,11 +4007,11 @@
         <v>0.99960000000000004</v>
       </c>
       <c r="V4" s="77">
-        <f>0.001*O4*P4/Z4</f>
+        <f t="shared" ref="V4:V17" si="1">0.001*O4*P4/Z4</f>
         <v>4342.4277478881349</v>
       </c>
       <c r="W4" s="78">
-        <f>Y4*0.01*P4/(O4*0.001)</f>
+        <f t="shared" ref="W4:W17" si="2">Y4*0.01*P4/(O4*0.001)</f>
         <v>0.58641540700282957</v>
       </c>
       <c r="X4" s="5">
@@ -4034,19 +4024,19 @@
         <v>1.5999999999999999E-5</v>
       </c>
       <c r="AA4" s="66">
-        <f t="shared" ref="AA4:AA17" si="0">100*K4/(287*N4)</f>
+        <f t="shared" ref="AA4:AA17" si="3">100*K4/(287*N4)</f>
         <v>118.84543954677628</v>
       </c>
       <c r="AB4" s="67">
-        <f t="shared" ref="AB4:AB17" si="1">SQRT(2000000*Z4/Y4)</f>
+        <f t="shared" ref="AB4:AB17" si="4">SQRT(2000000*Z4/Y4)</f>
         <v>9.5618288746751485</v>
       </c>
       <c r="AC4" s="68">
-        <f>AB4/P4</f>
+        <f t="shared" ref="AC4:AC17" si="5">AB4/P4</f>
         <v>2.8025025164698452</v>
       </c>
-      <c r="AD4" s="153"/>
-      <c r="AE4" s="154"/>
+      <c r="AD4" s="143"/>
+      <c r="AE4" s="144"/>
     </row>
     <row r="5" spans="1:31" ht="15.75">
       <c r="A5" s="43"/>
@@ -4102,22 +4092,22 @@
         <v>13.407681428571431</v>
       </c>
       <c r="S5" s="137">
-        <f>R5/H5</f>
+        <f t="shared" si="0"/>
         <v>0.7942939234935682</v>
       </c>
-      <c r="T5" s="151">
-        <f t="shared" ref="T5:T68" si="2">(H5-R5)/P5</f>
+      <c r="T5" s="141">
+        <f t="shared" ref="T5:T68" si="6">(H5-R5)/P5</f>
         <v>0.8948149054713308</v>
       </c>
       <c r="U5" s="121">
         <v>0.99939999999999996</v>
       </c>
       <c r="V5" s="79">
-        <f>0.001*O5*P5/Z5</f>
+        <f t="shared" si="1"/>
         <v>4133.1125755939147</v>
       </c>
       <c r="W5" s="80">
-        <f>Y5*0.01*P5/(O5*0.001)</f>
+        <f t="shared" si="2"/>
         <v>0.74915449113685773</v>
       </c>
       <c r="X5" s="7">
@@ -4130,15 +4120,15 @@
         <v>1.5999999999999999E-5</v>
       </c>
       <c r="AA5" s="63">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>119.33637220466981</v>
       </c>
       <c r="AB5" s="60">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>9.862273454430758</v>
       </c>
       <c r="AC5" s="69">
-        <f>AB5/P5</f>
+        <f t="shared" si="5"/>
         <v>2.5415033521040562</v>
       </c>
     </row>
@@ -4196,22 +4186,22 @@
         <v>15.814930612244902</v>
       </c>
       <c r="S6" s="137">
-        <f>R6/H6</f>
+        <f t="shared" si="0"/>
         <v>0.81394393269402487</v>
       </c>
-      <c r="T6" s="151">
-        <f t="shared" si="2"/>
+      <c r="T6" s="141">
+        <f t="shared" si="6"/>
         <v>0.81864871134984973</v>
       </c>
       <c r="U6" s="121">
         <v>0.999</v>
       </c>
       <c r="V6" s="79">
-        <f>0.001*O6*P6/Z6</f>
+        <f t="shared" si="1"/>
         <v>4973.6641603004728</v>
       </c>
       <c r="W6" s="80">
-        <f>Y6*0.01*P6/(O6*0.001)</f>
+        <f t="shared" si="2"/>
         <v>0.80619030022618976</v>
       </c>
       <c r="X6" s="7">
@@ -4224,15 +4214,15 @@
         <v>1.5999999999999999E-5</v>
       </c>
       <c r="AA6" s="63">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>119.32468573625628</v>
       </c>
       <c r="AB6" s="60">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>9.862273454430758</v>
       </c>
       <c r="AC6" s="69">
-        <f>AB6/P6</f>
+        <f t="shared" si="5"/>
         <v>2.2333561512807467</v>
       </c>
     </row>
@@ -4292,22 +4282,22 @@
         <v>16.981679999999997</v>
       </c>
       <c r="S7" s="137">
-        <f>R7/H7</f>
+        <f t="shared" si="0"/>
         <v>0.80634757834757831</v>
       </c>
-      <c r="T7" s="151">
-        <f t="shared" si="2"/>
+      <c r="T7" s="141">
+        <f t="shared" si="6"/>
         <v>0.85982190484636556</v>
       </c>
       <c r="U7" s="121">
         <v>0.99780000000000002</v>
       </c>
       <c r="V7" s="79">
-        <f>0.001*O7*P7/Z7</f>
+        <f t="shared" si="1"/>
         <v>4414.9746590256291</v>
       </c>
       <c r="W7" s="80">
-        <f>Y7*0.01*P7/(O7*0.001)</f>
+        <f t="shared" si="2"/>
         <v>1.0319113768534312</v>
       </c>
       <c r="X7" s="7">
@@ -4320,15 +4310,15 @@
         <v>1.5999999999999999E-5</v>
       </c>
       <c r="AA7" s="63">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>119.11907882801295</v>
       </c>
       <c r="AB7" s="60">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>9.9380798999990656</v>
       </c>
       <c r="AC7" s="69">
-        <f>AB7/P7</f>
+        <f t="shared" si="5"/>
         <v>2.0952202843652707</v>
       </c>
     </row>
@@ -4386,22 +4376,22 @@
         <v>18.445866279069776</v>
       </c>
       <c r="S8" s="137">
-        <f>R8/H8</f>
+        <f t="shared" si="0"/>
         <v>0.79473788363075293</v>
       </c>
-      <c r="T8" s="151">
-        <f t="shared" si="2"/>
+      <c r="T8" s="141">
+        <f t="shared" si="6"/>
         <v>0.89466561764813812</v>
       </c>
       <c r="U8" s="121">
         <v>0.99880000000000002</v>
       </c>
       <c r="V8" s="79">
-        <f>0.001*O8*P8/Z8</f>
+        <f t="shared" si="1"/>
         <v>5415.7674708868517</v>
       </c>
       <c r="W8" s="80">
-        <f>Y8*0.01*P8/(O8*0.001)</f>
+        <f t="shared" si="2"/>
         <v>1.0602576356248203</v>
       </c>
       <c r="X8" s="7">
@@ -4414,15 +4404,15 @@
         <v>1.5999999999999999E-5</v>
       </c>
       <c r="AA8" s="63">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>119.11557875713652</v>
       </c>
       <c r="AB8" s="60">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>9.9380798999990656</v>
       </c>
       <c r="AC8" s="69">
-        <f>AB8/P8</f>
+        <f t="shared" si="5"/>
         <v>1.8662906863649369</v>
       </c>
     </row>
@@ -4480,22 +4470,22 @@
         <v>19.509380722891567</v>
       </c>
       <c r="S9" s="137">
-        <f>R9/H9</f>
+        <f t="shared" si="0"/>
         <v>0.78476994058292715</v>
       </c>
-      <c r="T9" s="151">
-        <f t="shared" si="2"/>
+      <c r="T9" s="141">
+        <f t="shared" si="6"/>
         <v>0.97191992245242664</v>
       </c>
       <c r="U9" s="121">
         <v>0.99819999999999998</v>
       </c>
       <c r="V9" s="79">
-        <f>0.001*O9*P9/Z9</f>
+        <f t="shared" si="1"/>
         <v>5450.814992424087</v>
       </c>
       <c r="W9" s="80">
-        <f>Y9*0.01*P9/(O9*0.001)</f>
+        <f t="shared" si="2"/>
         <v>1.1259282521968137</v>
       </c>
       <c r="X9" s="7">
@@ -4508,15 +4498,15 @@
         <v>1.5999999999999999E-5</v>
       </c>
       <c r="AA9" s="63">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>119.11091199596794</v>
       </c>
       <c r="AB9" s="60">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>9.9380798999990656</v>
       </c>
       <c r="AC9" s="69">
-        <f>AB9/P9</f>
+        <f t="shared" si="5"/>
         <v>1.8052149378404312</v>
       </c>
     </row>
@@ -4574,22 +4564,22 @@
         <v>21.74608928571428</v>
       </c>
       <c r="S10" s="137">
-        <f>R10/H10</f>
+        <f t="shared" si="0"/>
         <v>0.80481455535582092</v>
       </c>
-      <c r="T10" s="151">
-        <f t="shared" si="2"/>
+      <c r="T10" s="141">
+        <f t="shared" si="6"/>
         <v>0.89587599055044254</v>
       </c>
       <c r="U10" s="121">
         <v>0.99760000000000004</v>
       </c>
       <c r="V10" s="79">
-        <f>0.001*O10*P10/Z10</f>
+        <f t="shared" si="1"/>
         <v>7299.1552273008219</v>
       </c>
       <c r="W10" s="80">
-        <f>Y10*0.01*P10/(O10*0.001)</f>
+        <f t="shared" si="2"/>
         <v>0.96143998223507865</v>
       </c>
       <c r="X10" s="7">
@@ -4602,15 +4592,15 @@
         <v>1.5999999999999999E-5</v>
       </c>
       <c r="AA10" s="63">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>119.10974530567579</v>
       </c>
       <c r="AB10" s="60">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>9.9380798999990656</v>
       </c>
       <c r="AC10" s="69">
-        <f>AB10/P10</f>
+        <f t="shared" si="5"/>
         <v>1.6881755602089175</v>
       </c>
     </row>
@@ -4668,22 +4658,22 @@
         <v>24.425961971830986</v>
       </c>
       <c r="S11" s="137">
-        <f>R11/H11</f>
+        <f t="shared" si="0"/>
         <v>0.83880363914254763</v>
       </c>
-      <c r="T11" s="151">
-        <f t="shared" si="2"/>
+      <c r="T11" s="141">
+        <f t="shared" si="6"/>
         <v>0.67818894104795147</v>
       </c>
       <c r="U11" s="121">
         <v>0.99870000000000003</v>
       </c>
       <c r="V11" s="79">
-        <f>0.001*O11*P11/Z11</f>
+        <f t="shared" si="1"/>
         <v>8391.2058643290129</v>
       </c>
       <c r="W11" s="80">
-        <f>Y11*0.01*P11/(O11*0.001)</f>
+        <f t="shared" si="2"/>
         <v>1.1560921483898943</v>
       </c>
       <c r="X11" s="7">
@@ -4696,15 +4686,15 @@
         <v>1.5999999999999999E-5</v>
       </c>
       <c r="AA11" s="63">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>119.09574502217005</v>
       </c>
       <c r="AB11" s="60">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>9.9380798999990656</v>
       </c>
       <c r="AC11" s="69">
-        <f>AB11/P11</f>
+        <f t="shared" si="5"/>
         <v>1.435841772687833</v>
       </c>
     </row>
@@ -4762,22 +4752,22 @@
         <v>25.46865714285715</v>
       </c>
       <c r="S12" s="137">
-        <f>R12/H12</f>
+        <f t="shared" si="0"/>
         <v>0.82529673178409435</v>
       </c>
-      <c r="T12" s="151">
-        <f t="shared" si="2"/>
+      <c r="T12" s="141">
+        <f t="shared" si="6"/>
         <v>0.74596603988193166</v>
       </c>
       <c r="U12" s="121">
         <v>0.998</v>
       </c>
       <c r="V12" s="79">
-        <f>0.001*O12*P12/Z12</f>
+        <f t="shared" si="1"/>
         <v>9164.0379753587276</v>
       </c>
       <c r="W12" s="80">
-        <f>Y12*0.01*P12/(O12*0.001)</f>
+        <f t="shared" si="2"/>
         <v>1.1542341951269097</v>
       </c>
       <c r="X12" s="7">
@@ -4790,15 +4780,15 @@
         <v>1.5999999999999999E-5</v>
       </c>
       <c r="AA12" s="63">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>119.06074431340569</v>
       </c>
       <c r="AB12" s="60">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>9.9380798999990656</v>
       </c>
       <c r="AC12" s="69">
-        <f>AB12/P12</f>
+        <f t="shared" si="5"/>
         <v>1.3750693108323864</v>
       </c>
     </row>
@@ -4858,22 +4848,22 @@
         <v>26.343295238095237</v>
       </c>
       <c r="S13" s="138">
-        <f>R13/H13</f>
+        <f t="shared" si="0"/>
         <v>0.79876577435097751</v>
       </c>
-      <c r="T13" s="152">
-        <f t="shared" si="2"/>
+      <c r="T13" s="142">
+        <f t="shared" si="6"/>
         <v>0.90268422472955046</v>
       </c>
       <c r="U13" s="122">
         <v>0.99790000000000001</v>
       </c>
       <c r="V13" s="81">
-        <f>0.001*O13*P13/Z13</f>
+        <f t="shared" si="1"/>
         <v>8289.8548207536496</v>
       </c>
       <c r="W13" s="82">
-        <f>Y13*0.01*P13/(O13*0.001)</f>
+        <f t="shared" si="2"/>
         <v>1.4263773293344597</v>
       </c>
       <c r="X13" s="24">
@@ -4886,15 +4876,15 @@
         <v>1.5999999999999999E-5</v>
       </c>
       <c r="AA13" s="72">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>118.86640487187567</v>
       </c>
       <c r="AB13" s="73">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>9.5618288746751485</v>
       </c>
       <c r="AC13" s="74">
-        <f>AB13/P13</f>
+        <f t="shared" si="5"/>
         <v>1.3005418192289071</v>
       </c>
     </row>
@@ -4952,20 +4942,20 @@
         <v>12.774771250000002</v>
       </c>
       <c r="S14" s="136">
-        <f>R14/H14</f>
+        <f t="shared" si="0"/>
         <v>0.83659274721676513</v>
       </c>
-      <c r="T14" s="150">
-        <f t="shared" si="2"/>
+      <c r="T14" s="140">
+        <f t="shared" si="6"/>
         <v>0.6917369040750061</v>
       </c>
       <c r="U14" s="18"/>
       <c r="V14" s="77">
-        <f>0.001*O14*P14/Z14</f>
+        <f t="shared" si="1"/>
         <v>4490.7427065550055</v>
       </c>
       <c r="W14" s="78">
-        <f>Y14*0.01*P14/(O14*0.001)</f>
+        <f t="shared" si="2"/>
         <v>0.56500888568509988</v>
       </c>
       <c r="X14" s="3">
@@ -4978,19 +4968,19 @@
         <v>1.5999999999999999E-5</v>
       </c>
       <c r="AA14" s="66">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>118.24953064221236</v>
       </c>
       <c r="AB14" s="67">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>10.127393670836666</v>
       </c>
       <c r="AC14" s="68">
-        <f>AB14/P14</f>
+        <f t="shared" si="5"/>
         <v>2.8075549963959716</v>
       </c>
-      <c r="AD14" s="153"/>
-      <c r="AE14" s="154"/>
+      <c r="AD14" s="143"/>
+      <c r="AE14" s="144"/>
     </row>
     <row r="15" spans="1:31" ht="15.75">
       <c r="A15" s="45"/>
@@ -5046,20 +5036,20 @@
         <v>13.62300294117647</v>
       </c>
       <c r="S15" s="137">
-        <f>R15/H15</f>
+        <f t="shared" si="0"/>
         <v>0.80657211019398867</v>
       </c>
-      <c r="T15" s="151">
-        <f t="shared" si="2"/>
+      <c r="T15" s="141">
+        <f t="shared" si="6"/>
         <v>0.80946323635297623</v>
       </c>
       <c r="U15" s="32"/>
       <c r="V15" s="79">
-        <f>0.001*O15*P15/Z15</f>
+        <f t="shared" si="1"/>
         <v>5010.8524700093503</v>
       </c>
       <c r="W15" s="80">
-        <f>Y15*0.01*P15/(O15*0.001)</f>
+        <f t="shared" si="2"/>
         <v>0.63390798716127184</v>
       </c>
       <c r="X15" s="7">
@@ -5072,15 +5062,15 @@
         <v>1.5999999999999999E-5</v>
       </c>
       <c r="AA15" s="63">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>118.28809598797697</v>
       </c>
       <c r="AB15" s="60">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>10.127393670836666</v>
       </c>
       <c r="AC15" s="69">
-        <f>AB15/P15</f>
+        <f t="shared" si="5"/>
         <v>2.5092623926536883</v>
       </c>
     </row>
@@ -5138,20 +5128,20 @@
         <v>15.366440229885058</v>
       </c>
       <c r="S16" s="137">
-        <f>R16/H16</f>
+        <f t="shared" si="0"/>
         <v>0.80748503572701291</v>
       </c>
-      <c r="T16" s="151">
-        <f t="shared" si="2"/>
+      <c r="T16" s="141">
+        <f t="shared" si="6"/>
         <v>0.85169028646124112</v>
       </c>
       <c r="U16" s="32"/>
       <c r="V16" s="79">
-        <f>0.001*O16*P16/Z16</f>
+        <f t="shared" si="1"/>
         <v>4684.9838727966253</v>
       </c>
       <c r="W16" s="80">
-        <f>Y16*0.01*P16/(O16*0.001)</f>
+        <f t="shared" si="2"/>
         <v>0.77014000868690335</v>
       </c>
       <c r="X16" s="7">
@@ -5164,15 +5154,15 @@
         <v>1.5999999999999999E-5</v>
       </c>
       <c r="AA16" s="63">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>118.28926463481832</v>
       </c>
       <c r="AB16" s="60">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>10.127393670836666</v>
       </c>
       <c r="AC16" s="69">
-        <f>AB16/P16</f>
+        <f t="shared" si="5"/>
         <v>2.3543775338350819</v>
       </c>
     </row>
@@ -5230,20 +5220,20 @@
         <v>17.517375362318838</v>
       </c>
       <c r="S17" s="137">
-        <f>R17/H17</f>
+        <f t="shared" si="0"/>
         <v>0.8290286494235134</v>
       </c>
-      <c r="T17" s="151">
-        <f t="shared" si="2"/>
+      <c r="T17" s="141">
+        <f t="shared" si="6"/>
         <v>0.7641829034540577</v>
       </c>
       <c r="U17" s="32"/>
       <c r="V17" s="79">
-        <f>0.001*O17*P17/Z17</f>
+        <f t="shared" si="1"/>
         <v>6351.3913390510852</v>
       </c>
       <c r="W17" s="80">
-        <f>Y17*0.01*P17/(O17*0.001)</f>
+        <f t="shared" si="2"/>
         <v>0.72353257224129963</v>
       </c>
       <c r="X17" s="7">
@@ -5256,15 +5246,15 @@
         <v>1.5999999999999999E-5</v>
       </c>
       <c r="AA17" s="63">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>118.25069928905371</v>
       </c>
       <c r="AB17" s="60">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>9.862273454430758</v>
       </c>
       <c r="AC17" s="69">
-        <f>AB17/P17</f>
+        <f t="shared" si="5"/>
         <v>2.0861787533792295</v>
       </c>
       <c r="AD17">
@@ -5329,11 +5319,11 @@
         <v>20.324461538461602</v>
       </c>
       <c r="S18" s="137">
-        <f>R18/H18</f>
+        <f t="shared" si="0"/>
         <v>0.87567692970536848</v>
       </c>
-      <c r="T18" s="151">
-        <f t="shared" si="2"/>
+      <c r="T18" s="141">
+        <f t="shared" si="6"/>
         <v>0.89489520353766505</v>
       </c>
       <c r="U18" s="32"/>
@@ -5345,7 +5335,7 @@
       <c r="AA18" s="63"/>
       <c r="AB18" s="60"/>
       <c r="AC18" s="69"/>
-      <c r="AD18" s="139" t="s">
+      <c r="AD18" s="145" t="s">
         <v>63</v>
       </c>
     </row>
@@ -5403,20 +5393,20 @@
         <v>21.16130714285714</v>
       </c>
       <c r="S19" s="137">
-        <f>R19/H19</f>
+        <f t="shared" si="0"/>
         <v>0.83443640153222165</v>
       </c>
-      <c r="T19" s="151">
-        <f t="shared" si="2"/>
+      <c r="T19" s="141">
+        <f t="shared" si="6"/>
         <v>0.70872232162054016</v>
       </c>
       <c r="U19" s="32"/>
       <c r="V19" s="79">
-        <f>0.001*O19*P19/Z19</f>
+        <f t="shared" ref="V19:V41" si="7">0.001*O19*P19/Z19</f>
         <v>8925.8132156772062</v>
       </c>
       <c r="W19" s="80">
-        <f>Y19*0.01*P19/(O19*0.001)</f>
+        <f t="shared" ref="W19:W41" si="8">Y19*0.01*P19/(O19*0.001)</f>
         <v>0.73973251473866286</v>
       </c>
       <c r="X19" s="7">
@@ -5429,18 +5419,18 @@
         <v>1.5999999999999999E-5</v>
       </c>
       <c r="AA19" s="63">
-        <f t="shared" ref="AA19:AA41" si="3">100*K19/(287*N19)</f>
+        <f t="shared" ref="AA19:AA41" si="9">100*K19/(287*N19)</f>
         <v>118.07456259166193</v>
       </c>
       <c r="AB19" s="60">
-        <f t="shared" ref="AB19:AB41" si="4">SQRT(2000000*Z19/Y19)</f>
+        <f t="shared" ref="AB19:AB41" si="10">SQRT(2000000*Z19/Y19)</f>
         <v>10.310785244529342</v>
       </c>
       <c r="AC19" s="69">
-        <f>AB19/P19</f>
+        <f t="shared" ref="AC19:AC41" si="11">AB19/P19</f>
         <v>1.7404187219367757</v>
       </c>
-      <c r="AD19" s="139"/>
+      <c r="AD19" s="145"/>
     </row>
     <row r="20" spans="1:31" ht="15.75">
       <c r="A20" s="43"/>
@@ -5496,20 +5486,20 @@
         <v>22.203826851851854</v>
       </c>
       <c r="S20" s="137">
-        <f>R20/H20</f>
+        <f t="shared" si="0"/>
         <v>0.82145123388279151</v>
       </c>
-      <c r="T20" s="151">
-        <f t="shared" si="2"/>
+      <c r="T20" s="141">
+        <f t="shared" si="6"/>
         <v>0.77608017192253564</v>
       </c>
       <c r="U20" s="32"/>
       <c r="V20" s="79">
-        <f>0.001*O20*P20/Z20</f>
+        <f t="shared" si="7"/>
         <v>7284.4892987893245</v>
       </c>
       <c r="W20" s="80">
-        <f>Y20*0.01*P20/(O20*0.001)</f>
+        <f t="shared" si="8"/>
         <v>1.0153013335278926</v>
       </c>
       <c r="X20" s="7">
@@ -5522,18 +5512,18 @@
         <v>1.5999999999999999E-5</v>
       </c>
       <c r="AA20" s="63">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>117.97572234171076</v>
       </c>
       <c r="AB20" s="60">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>10.226199851298272</v>
       </c>
       <c r="AC20" s="69">
-        <f>AB20/P20</f>
+        <f t="shared" si="11"/>
         <v>1.6444397445116599</v>
       </c>
-      <c r="AD20" s="139"/>
+      <c r="AD20" s="145"/>
     </row>
     <row r="21" spans="1:31" ht="15.75">
       <c r="A21" s="43"/>
@@ -5589,20 +5579,20 @@
         <v>23.381500000000006</v>
       </c>
       <c r="S21" s="137">
-        <f>R21/H21</f>
+        <f t="shared" si="0"/>
         <v>0.80293612637362655</v>
       </c>
-      <c r="T21" s="151">
-        <f t="shared" si="2"/>
+      <c r="T21" s="141">
+        <f t="shared" si="6"/>
         <v>0.87957615109057519</v>
       </c>
       <c r="U21" s="32"/>
       <c r="V21" s="79">
-        <f>0.001*O21*P21/Z21</f>
+        <f t="shared" si="7"/>
         <v>7120.5964844444397</v>
       </c>
       <c r="W21" s="80">
-        <f>Y21*0.01*P21/(O21*0.001)</f>
+        <f t="shared" si="8"/>
         <v>1.1096090045149969</v>
       </c>
       <c r="X21" s="7">
@@ -5615,15 +5605,15 @@
         <v>1.5999999999999999E-5</v>
       </c>
       <c r="AA21" s="63">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>118.15720754174554</v>
       </c>
       <c r="AB21" s="60">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>10.37998592215364</v>
       </c>
       <c r="AC21" s="69">
-        <f>AB21/P21</f>
+        <f t="shared" si="11"/>
         <v>1.5910060234873682</v>
       </c>
     </row>
@@ -5681,20 +5671,20 @@
         <v>25.011321839080463</v>
       </c>
       <c r="S22" s="137">
-        <f>R22/H22</f>
+        <f t="shared" si="0"/>
         <v>0.81021450725884225</v>
       </c>
-      <c r="T22" s="151">
-        <f t="shared" si="2"/>
+      <c r="T22" s="141">
+        <f t="shared" si="6"/>
         <v>0.87576349734397207</v>
       </c>
       <c r="U22" s="32"/>
       <c r="V22" s="79">
-        <f>0.001*O22*P22/Z22</f>
+        <f t="shared" si="7"/>
         <v>7154.6603580106494</v>
       </c>
       <c r="W22" s="80">
-        <f>Y22*0.01*P22/(O22*0.001)</f>
+        <f t="shared" si="8"/>
         <v>1.1611091521624624</v>
       </c>
       <c r="X22" s="7">
@@ -5707,15 +5697,15 @@
         <v>1.5999999999999999E-5</v>
       </c>
       <c r="AA22" s="63">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>118.1607134822696</v>
       </c>
       <c r="AB22" s="60">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>10.37998592215364</v>
       </c>
       <c r="AC22" s="69">
-        <f>AB22/P22</f>
+        <f t="shared" si="11"/>
         <v>1.5516149759179974</v>
       </c>
     </row>
@@ -5773,20 +5763,20 @@
         <v>28.333817708333342</v>
       </c>
       <c r="S23" s="138">
-        <f>R23/H23</f>
+        <f t="shared" si="0"/>
         <v>0.8485719589198365</v>
       </c>
-      <c r="T23" s="152">
-        <f t="shared" si="2"/>
+      <c r="T23" s="142">
+        <f t="shared" si="6"/>
         <v>0.69062689082979856</v>
       </c>
       <c r="U23" s="33"/>
       <c r="V23" s="81">
-        <f>0.001*O23*P23/Z23</f>
+        <f t="shared" si="7"/>
         <v>10029.982578744082</v>
       </c>
       <c r="W23" s="82">
-        <f>Y23*0.01*P23/(O23*0.001)</f>
+        <f t="shared" si="8"/>
         <v>0.99196138368212661</v>
       </c>
       <c r="X23" s="23">
@@ -5799,15 +5789,15 @@
         <v>1.5999999999999999E-5</v>
       </c>
       <c r="AA23" s="72">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>118.15136430753878</v>
       </c>
       <c r="AB23" s="73">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>10.37998592215364</v>
       </c>
       <c r="AC23" s="74">
-        <f>AB23/P23</f>
+        <f t="shared" si="11"/>
         <v>1.4178083365564429</v>
       </c>
     </row>
@@ -5865,20 +5855,20 @@
         <v>12.587934751773052</v>
       </c>
       <c r="S24" s="136">
-        <f>R24/H24</f>
+        <f t="shared" si="0"/>
         <v>0.8281536020903324</v>
       </c>
-      <c r="T24" s="150">
-        <f t="shared" si="2"/>
+      <c r="T24" s="140">
+        <f t="shared" si="6"/>
         <v>0.72412404292989685</v>
       </c>
       <c r="U24" s="18"/>
       <c r="V24" s="77">
-        <f>0.001*O24*P24/Z24</f>
+        <f t="shared" si="7"/>
         <v>4396.7755592026815</v>
       </c>
       <c r="W24" s="78">
-        <f>Y24*0.01*P24/(O24*0.001)</f>
+        <f t="shared" si="8"/>
         <v>0.54564457778941522</v>
       </c>
       <c r="X24" s="3">
@@ -5891,19 +5881,19 @@
         <v>1.5999999999999999E-5</v>
       </c>
       <c r="AA24" s="66">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>117.84673885547824</v>
       </c>
       <c r="AB24" s="67">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>10.41511287846591</v>
       </c>
       <c r="AC24" s="68">
-        <f>AB24/P24</f>
+        <f t="shared" si="11"/>
         <v>2.8873067586061705</v>
       </c>
-      <c r="AD24" s="153"/>
-      <c r="AE24" s="154"/>
+      <c r="AD24" s="143"/>
+      <c r="AE24" s="144"/>
     </row>
     <row r="25" spans="1:31" ht="15.75">
       <c r="A25" s="43"/>
@@ -5959,20 +5949,20 @@
         <v>13.902478651685401</v>
       </c>
       <c r="S25" s="137">
-        <f>R25/H25</f>
+        <f t="shared" si="0"/>
         <v>0.80500744943169666</v>
       </c>
-      <c r="T25" s="151">
-        <f t="shared" si="2"/>
+      <c r="T25" s="141">
+        <f t="shared" si="6"/>
         <v>0.85841550728914506</v>
       </c>
       <c r="U25" s="32"/>
       <c r="V25" s="79">
-        <f>0.001*O25*P25/Z25</f>
+        <f t="shared" si="7"/>
         <v>3987.1799519458154</v>
       </c>
       <c r="W25" s="80">
-        <f>Y25*0.01*P25/(O25*0.001)</f>
+        <f t="shared" si="8"/>
         <v>0.71164237833376165</v>
       </c>
       <c r="X25" s="7">
@@ -5985,15 +5975,15 @@
         <v>1.5999999999999999E-5</v>
       </c>
       <c r="AA25" s="63">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>117.85373314231161</v>
       </c>
       <c r="AB25" s="60">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>10.41511287846591</v>
       </c>
       <c r="AC25" s="69">
-        <f>AB25/P25</f>
+        <f t="shared" si="11"/>
         <v>2.6549184044569238</v>
       </c>
     </row>
@@ -6051,20 +6041,20 @@
         <v>16.209973469387755</v>
       </c>
       <c r="S26" s="137">
-        <f>R26/H26</f>
+        <f t="shared" si="0"/>
         <v>0.83729201804688824</v>
       </c>
-      <c r="T26" s="151">
-        <f t="shared" si="2"/>
+      <c r="T26" s="141">
+        <f t="shared" si="6"/>
         <v>0.72122636936278017</v>
       </c>
       <c r="U26" s="32"/>
       <c r="V26" s="79">
-        <f>0.001*O26*P26/Z26</f>
+        <f t="shared" si="7"/>
         <v>5428.5645221763671</v>
       </c>
       <c r="W26" s="80">
-        <f>Y26*0.01*P26/(O26*0.001)</f>
+        <f t="shared" si="8"/>
         <v>0.66985388710159288</v>
       </c>
       <c r="X26" s="7">
@@ -6077,15 +6067,15 @@
         <v>1.5999999999999999E-5</v>
       </c>
       <c r="AA26" s="63">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>117.95472191645216</v>
       </c>
       <c r="AB26" s="60">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>10.242950394631679</v>
       </c>
       <c r="AC26" s="69">
-        <f>AB26/P26</f>
+        <f t="shared" si="11"/>
         <v>2.3452138745153421</v>
       </c>
     </row>
@@ -6143,20 +6133,20 @@
         <v>17.93944545454546</v>
       </c>
       <c r="S27" s="137">
-        <f>R27/H27</f>
+        <f t="shared" si="0"/>
         <v>0.8506138195611882</v>
       </c>
-      <c r="T27" s="151">
-        <f t="shared" si="2"/>
+      <c r="T27" s="141">
+        <f t="shared" si="6"/>
         <v>0.67346162104040563</v>
       </c>
       <c r="U27" s="32"/>
       <c r="V27" s="79">
-        <f>0.001*O27*P27/Z27</f>
+        <f t="shared" si="7"/>
         <v>5927.4107589204214</v>
       </c>
       <c r="W27" s="80">
-        <f>Y27*0.01*P27/(O27*0.001)</f>
+        <f t="shared" si="8"/>
         <v>0.66228541820928821</v>
       </c>
       <c r="X27" s="7">
@@ -6169,15 +6159,15 @@
         <v>1.5999999999999999E-5</v>
       </c>
       <c r="AA27" s="63">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>118.03719722375318</v>
       </c>
       <c r="AB27" s="60">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>10.559273546969093</v>
       </c>
       <c r="AC27" s="69">
-        <f>AB27/P27</f>
+        <f t="shared" si="11"/>
         <v>2.25714723467037</v>
       </c>
     </row>
@@ -6235,20 +6225,20 @@
         <v>19.18855051546392</v>
       </c>
       <c r="S28" s="137">
-        <f>R28/H28</f>
+        <f t="shared" si="0"/>
         <v>0.82887907194228605</v>
       </c>
-      <c r="T28" s="151">
-        <f t="shared" si="2"/>
+      <c r="T28" s="141">
+        <f t="shared" si="6"/>
         <v>0.82511745021720706</v>
       </c>
       <c r="U28" s="32"/>
       <c r="V28" s="79">
-        <f>0.001*O28*P28/Z28</f>
+        <f t="shared" si="7"/>
         <v>5343.4285381607888</v>
       </c>
       <c r="W28" s="80">
-        <f>Y28*0.01*P28/(O28*0.001)</f>
+        <f t="shared" si="8"/>
         <v>0.77378197546759941</v>
       </c>
       <c r="X28" s="7">
@@ -6261,15 +6251,15 @@
         <v>1.5999999999999999E-5</v>
       </c>
       <c r="AA28" s="63">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>118.02668821402884</v>
       </c>
       <c r="AB28" s="60">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>10.559273546969093</v>
       </c>
       <c r="AC28" s="69">
-        <f>AB28/P28</f>
+        <f t="shared" si="11"/>
         <v>2.1993568008961928</v>
       </c>
     </row>
@@ -6327,20 +6317,20 @@
         <v>20.230562499999998</v>
       </c>
       <c r="S29" s="137">
-        <f>R29/H29</f>
+        <f t="shared" si="0"/>
         <v>0.81377966613032982</v>
       </c>
-      <c r="T29" s="151">
-        <f t="shared" si="2"/>
+      <c r="T29" s="141">
+        <f t="shared" si="6"/>
         <v>0.7740533636518373</v>
       </c>
       <c r="U29" s="32"/>
       <c r="V29" s="79">
-        <f>0.001*O29*P29/Z29</f>
+        <f t="shared" si="7"/>
         <v>7115.6701380646628</v>
       </c>
       <c r="W29" s="80">
-        <f>Y29*0.01*P29/(O29*0.001)</f>
+        <f t="shared" si="8"/>
         <v>0.93625709165545234</v>
       </c>
       <c r="X29" s="7">
@@ -6353,15 +6343,15 @@
         <v>1.5999999999999999E-5</v>
       </c>
       <c r="AA29" s="63">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>117.90805430476635</v>
       </c>
       <c r="AB29" s="60">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>10.362555203016797</v>
       </c>
       <c r="AC29" s="69">
-        <f>AB29/P29</f>
+        <f t="shared" si="11"/>
         <v>1.7326447783176675</v>
       </c>
     </row>
@@ -6419,20 +6409,20 @@
         <v>21.796570370370375</v>
       </c>
       <c r="S30" s="137">
-        <f>R30/H30</f>
+        <f t="shared" si="0"/>
         <v>0.80877812134955007</v>
       </c>
-      <c r="T30" s="151">
-        <f t="shared" si="2"/>
+      <c r="T30" s="141">
+        <f t="shared" si="6"/>
         <v>0.82371595340182968</v>
       </c>
       <c r="U30" s="32"/>
       <c r="V30" s="79">
-        <f>0.001*O30*P30/Z30</f>
+        <f t="shared" si="7"/>
         <v>6742.7144760951469</v>
       </c>
       <c r="W30" s="80">
-        <f>Y30*0.01*P30/(O30*0.001)</f>
+        <f t="shared" si="8"/>
         <v>1.1065800408212578</v>
       </c>
       <c r="X30" s="7">
@@ -6445,15 +6435,15 @@
         <v>1.5999999999999999E-5</v>
       </c>
       <c r="AA30" s="63">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>117.89872078242919</v>
       </c>
       <c r="AB30" s="60">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>10.242950394631679</v>
       </c>
       <c r="AC30" s="69">
-        <f>AB30/P30</f>
+        <f t="shared" si="11"/>
         <v>1.6372168160503371</v>
       </c>
     </row>
@@ -6511,20 +6501,20 @@
         <v>24.097979487179479</v>
       </c>
       <c r="S31" s="137">
-        <f>R31/H31</f>
+        <f t="shared" si="0"/>
         <v>0.82839393218217527</v>
       </c>
-      <c r="T31" s="151">
-        <f t="shared" si="2"/>
+      <c r="T31" s="141">
+        <f t="shared" si="6"/>
         <v>0.79443091328416204</v>
       </c>
       <c r="U31" s="32"/>
       <c r="V31" s="79">
-        <f>0.001*O31*P31/Z31</f>
+        <f t="shared" si="7"/>
         <v>6398.7312500281905</v>
       </c>
       <c r="W31" s="80">
-        <f>Y31*0.01*P31/(O31*0.001)</f>
+        <f t="shared" si="8"/>
         <v>1.1493250260041148</v>
       </c>
       <c r="X31" s="7">
@@ -6537,15 +6527,15 @@
         <v>1.5999999999999999E-5</v>
       </c>
       <c r="AA31" s="63">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>117.89522071155275</v>
       </c>
       <c r="AB31" s="60">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>10.362555203016797</v>
       </c>
       <c r="AC31" s="69">
-        <f>AB31/P31</f>
+        <f t="shared" si="11"/>
         <v>1.6490986310548756</v>
       </c>
     </row>
@@ -6603,20 +6593,20 @@
         <v>27.018077777777776</v>
       </c>
       <c r="S32" s="137">
-        <f>R32/H32</f>
+        <f t="shared" si="0"/>
         <v>0.86430191227696018</v>
       </c>
-      <c r="T32" s="151">
-        <f t="shared" si="2"/>
+      <c r="T32" s="141">
+        <f t="shared" si="6"/>
         <v>0.59897736952971425</v>
       </c>
       <c r="U32" s="32"/>
       <c r="V32" s="79">
-        <f>0.001*O32*P32/Z32</f>
+        <f t="shared" si="7"/>
         <v>9206.742504473028</v>
       </c>
       <c r="W32" s="80">
-        <f>Y32*0.01*P32/(O32*0.001)</f>
+        <f t="shared" si="8"/>
         <v>1.0146000012060898</v>
       </c>
       <c r="X32" s="7">
@@ -6629,15 +6619,15 @@
         <v>1.5999999999999999E-5</v>
       </c>
       <c r="AA32" s="63">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>117.90105416301348</v>
       </c>
       <c r="AB32" s="60">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>10.362555203016797</v>
       </c>
       <c r="AC32" s="69">
-        <f>AB32/P32</f>
+        <f t="shared" si="11"/>
         <v>1.4632366488459125</v>
       </c>
     </row>
@@ -6695,20 +6685,20 @@
         <v>28.536144444444453</v>
       </c>
       <c r="S33" s="138">
-        <f>R33/H33</f>
+        <f t="shared" si="0"/>
         <v>0.86630675301895732</v>
       </c>
-      <c r="T33" s="152">
-        <f t="shared" si="2"/>
+      <c r="T33" s="142">
+        <f t="shared" si="6"/>
         <v>0.59806342865964213</v>
       </c>
       <c r="U33" s="33"/>
       <c r="V33" s="81">
-        <f>0.001*O33*P33/Z33</f>
+        <f t="shared" si="7"/>
         <v>9670.1656267041471</v>
       </c>
       <c r="W33" s="82">
-        <f>Y33*0.01*P33/(O33*0.001)</f>
+        <f t="shared" si="8"/>
         <v>0.99175449941528127</v>
       </c>
       <c r="X33" s="23">
@@ -6721,15 +6711,15 @@
         <v>1.5999999999999999E-5</v>
       </c>
       <c r="AA33" s="72">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>118.06137850075467</v>
       </c>
       <c r="AB33" s="73">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>10.633635547027012</v>
       </c>
       <c r="AC33" s="74">
-        <f>AB33/P33</f>
+        <f t="shared" si="11"/>
         <v>1.4440956235154641</v>
       </c>
     </row>
@@ -6787,20 +6777,20 @@
         <v>11.99555154639175</v>
       </c>
       <c r="S34" s="136">
-        <f>R34/H34</f>
+        <f t="shared" si="0"/>
         <v>0.80723765453511109</v>
       </c>
-      <c r="T34" s="150">
-        <f t="shared" si="2"/>
+      <c r="T34" s="140">
+        <f t="shared" si="6"/>
         <v>0.83697137240455288</v>
       </c>
       <c r="U34" s="18"/>
       <c r="V34" s="77">
-        <f>0.001*O34*P34/Z34</f>
+        <f t="shared" si="7"/>
         <v>4139.7809283895085</v>
       </c>
       <c r="W34" s="78">
-        <f>Y34*0.01*P34/(O34*0.001)</f>
+        <f t="shared" si="8"/>
         <v>0.66772165158013874</v>
       </c>
       <c r="X34" s="3">
@@ -6813,19 +6803,19 @@
         <v>1.5E-5</v>
       </c>
       <c r="AA34" s="66">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>119.44483041859338</v>
       </c>
       <c r="AB34" s="67">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>9.2057461789832349</v>
       </c>
       <c r="AC34" s="68">
-        <f>AB34/P34</f>
+        <f t="shared" si="11"/>
         <v>2.6898532608348757</v>
       </c>
-      <c r="AD34" s="153"/>
-      <c r="AE34" s="154"/>
+      <c r="AD34" s="143"/>
+      <c r="AE34" s="144"/>
     </row>
     <row r="35" spans="1:31" ht="15.75">
       <c r="A35" s="43"/>
@@ -6881,20 +6871,20 @@
         <v>14.60224507042253</v>
       </c>
       <c r="S35" s="137">
-        <f>R35/H35</f>
+        <f t="shared" si="0"/>
         <v>0.83969206845442956</v>
       </c>
-      <c r="T35" s="151">
-        <f t="shared" si="2"/>
+      <c r="T35" s="141">
+        <f t="shared" si="6"/>
         <v>0.7520962484607594</v>
       </c>
       <c r="U35" s="32"/>
       <c r="V35" s="79">
-        <f>0.001*O35*P35/Z35</f>
+        <f t="shared" si="7"/>
         <v>4956.06928081159</v>
       </c>
       <c r="W35" s="80">
-        <f>Y35*0.01*P35/(O35*0.001)</f>
+        <f t="shared" si="8"/>
         <v>0.65423982098669675</v>
       </c>
       <c r="X35" s="7">
@@ -6907,15 +6897,15 @@
         <v>1.5E-5</v>
       </c>
       <c r="AA35" s="63">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>119.43310462166424</v>
       </c>
       <c r="AB35" s="60">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>9.2057461789832349</v>
       </c>
       <c r="AC35" s="69">
-        <f>AB35/P35</f>
+        <f t="shared" si="11"/>
         <v>2.4835781266270223</v>
       </c>
     </row>
@@ -6973,20 +6963,20 @@
         <v>16.152542045454545</v>
       </c>
       <c r="S36" s="137">
-        <f>R36/H36</f>
+        <f t="shared" si="0"/>
         <v>0.84656928959405386</v>
       </c>
-      <c r="T36" s="151">
-        <f t="shared" si="2"/>
+      <c r="T36" s="141">
+        <f t="shared" si="6"/>
         <v>0.72066602244063449</v>
       </c>
       <c r="U36" s="32"/>
       <c r="V36" s="79">
-        <f>0.001*O36*P36/Z36</f>
+        <f t="shared" si="7"/>
         <v>5265.4601544382831</v>
       </c>
       <c r="W36" s="80">
-        <f>Y36*0.01*P36/(O36*0.001)</f>
+        <f t="shared" si="8"/>
         <v>0.73958639152338723</v>
       </c>
       <c r="X36" s="7">
@@ -6999,15 +6989,15 @@
         <v>1.5E-5</v>
       </c>
       <c r="AA36" s="63">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>119.42372398412094</v>
       </c>
       <c r="AB36" s="60">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>9.2057461789832349</v>
       </c>
       <c r="AC36" s="69">
-        <f>AB36/P36</f>
+        <f t="shared" si="11"/>
         <v>2.2662216111780231</v>
       </c>
     </row>
@@ -7065,20 +7055,20 @@
         <v>17.683584466019418</v>
       </c>
       <c r="S37" s="137">
-        <f>R37/H37</f>
+        <f t="shared" si="0"/>
         <v>0.83689467420820729</v>
       </c>
-      <c r="T37" s="151">
-        <f t="shared" si="2"/>
+      <c r="T37" s="141">
+        <f t="shared" si="6"/>
         <v>0.79756625068217479</v>
       </c>
       <c r="U37" s="32"/>
       <c r="V37" s="79">
-        <f>0.001*O37*P37/Z37</f>
+        <f t="shared" si="7"/>
         <v>5762.1145701335099</v>
       </c>
       <c r="W37" s="80">
-        <f>Y37*0.01*P37/(O37*0.001)</f>
+        <f t="shared" si="8"/>
         <v>0.76477178189955997</v>
       </c>
       <c r="X37" s="7">
@@ -7091,15 +7081,15 @@
         <v>1.5E-5</v>
       </c>
       <c r="AA37" s="63">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>119.42137882473511</v>
       </c>
       <c r="AB37" s="60">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>9.2057461789832349</v>
       </c>
       <c r="AC37" s="69">
-        <f>AB37/P37</f>
+        <f t="shared" si="11"/>
         <v>2.1303851472092354</v>
       </c>
     </row>
@@ -7157,20 +7147,20 @@
         <v>19.153797916666669</v>
       </c>
       <c r="S38" s="137">
-        <f>R38/H38</f>
+        <f t="shared" si="0"/>
         <v>0.82240437598397031</v>
       </c>
-      <c r="T38" s="151">
-        <f t="shared" si="2"/>
+      <c r="T38" s="141">
+        <f t="shared" si="6"/>
         <v>0.86095099644913753</v>
       </c>
       <c r="U38" s="32"/>
       <c r="V38" s="79">
-        <f>0.001*O38*P38/Z38</f>
+        <f t="shared" si="7"/>
         <v>7031.4315999545352</v>
       </c>
       <c r="W38" s="80">
-        <f>Y38*0.01*P38/(O38*0.001)</f>
+        <f t="shared" si="8"/>
         <v>0.77466668376727865</v>
       </c>
       <c r="X38" s="7">
@@ -7183,15 +7173,15 @@
         <v>1.5E-5</v>
       </c>
       <c r="AA38" s="63">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>119.42020624504221</v>
       </c>
       <c r="AB38" s="60">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>9.2057461789832349</v>
       </c>
       <c r="AC38" s="69">
-        <f>AB38/P38</f>
+        <f t="shared" si="11"/>
         <v>1.9161772529900676</v>
       </c>
     </row>
@@ -7249,20 +7239,20 @@
         <v>20.131170000000001</v>
       </c>
       <c r="S39" s="137">
-        <f>R39/H39</f>
+        <f t="shared" si="0"/>
         <v>0.80589151321056851</v>
       </c>
-      <c r="T39" s="151">
-        <f t="shared" si="2"/>
+      <c r="T39" s="141">
+        <f t="shared" si="6"/>
         <v>0.84253239178559225</v>
       </c>
       <c r="U39" s="32"/>
       <c r="V39" s="79">
-        <f>0.001*O39*P39/Z39</f>
+        <f t="shared" si="7"/>
         <v>7338.8880134770634</v>
       </c>
       <c r="W39" s="80">
-        <f>Y39*0.01*P39/(O39*0.001)</f>
+        <f t="shared" si="8"/>
         <v>1.0349935077011203</v>
       </c>
       <c r="X39" s="7">
@@ -7275,15 +7265,15 @@
         <v>1.5E-5</v>
       </c>
       <c r="AA39" s="63">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>119.41551592627054</v>
       </c>
       <c r="AB39" s="60">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>9.3385920954703554</v>
       </c>
       <c r="AC39" s="69">
-        <f>AB39/P39</f>
+        <f t="shared" si="11"/>
         <v>1.6226731673633978</v>
       </c>
     </row>
@@ -7341,20 +7331,20 @@
         <v>22.172423437499997</v>
       </c>
       <c r="S40" s="137">
-        <f>R40/H40</f>
+        <f t="shared" si="0"/>
         <v>0.81847262596899217</v>
       </c>
-      <c r="T40" s="151">
-        <f t="shared" si="2"/>
+      <c r="T40" s="141">
+        <f t="shared" si="6"/>
         <v>0.82902337298704198</v>
       </c>
       <c r="U40" s="32"/>
       <c r="V40" s="79">
-        <f>0.001*O40*P40/Z40</f>
+        <f t="shared" si="7"/>
         <v>6639.3364897578576</v>
       </c>
       <c r="W40" s="80">
-        <f>Y40*0.01*P40/(O40*0.001)</f>
+        <f t="shared" si="8"/>
         <v>1.2153775621239993</v>
       </c>
       <c r="X40" s="7">
@@ -7367,15 +7357,15 @@
         <v>1.5E-5</v>
       </c>
       <c r="AA40" s="63">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>119.41903366534929</v>
       </c>
       <c r="AB40" s="60">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>9.3385920954703554</v>
       </c>
       <c r="AC40" s="69">
-        <f>AB40/P40</f>
+        <f t="shared" si="11"/>
         <v>1.574334638117179</v>
       </c>
     </row>
@@ -7433,20 +7423,20 @@
         <v>24.453162500000005</v>
       </c>
       <c r="S41" s="137">
-        <f>R41/H41</f>
+        <f t="shared" si="0"/>
         <v>0.84877342936480404</v>
       </c>
-      <c r="T41" s="151">
-        <f t="shared" si="2"/>
+      <c r="T41" s="141">
+        <f t="shared" si="6"/>
         <v>0.72440576605288132</v>
       </c>
       <c r="U41" s="32"/>
       <c r="V41" s="79">
-        <f>0.001*O41*P41/Z41</f>
+        <f t="shared" si="7"/>
         <v>8273.450248741301</v>
       </c>
       <c r="W41" s="80">
-        <f>Y41*0.01*P41/(O41*0.001)</f>
+        <f t="shared" si="8"/>
         <v>1.0026733013441613</v>
       </c>
       <c r="X41" s="7">
@@ -7459,15 +7449,15 @@
         <v>1.5E-5</v>
       </c>
       <c r="AA41" s="63">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>119.42489656381386</v>
       </c>
       <c r="AB41" s="60">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>9.3385920954703554</v>
       </c>
       <c r="AC41" s="69">
-        <f>AB41/P41</f>
+        <f t="shared" si="11"/>
         <v>1.5527156936136806</v>
       </c>
     </row>
@@ -7521,7 +7511,7 @@
       <c r="Q42" s="126"/>
       <c r="R42" s="137"/>
       <c r="S42" s="137"/>
-      <c r="T42" s="151"/>
+      <c r="T42" s="141"/>
       <c r="U42" s="96"/>
       <c r="V42" s="83"/>
       <c r="W42" s="86"/>
@@ -7582,7 +7572,7 @@
       <c r="Q43" s="126"/>
       <c r="R43" s="137"/>
       <c r="S43" s="137"/>
-      <c r="T43" s="151"/>
+      <c r="T43" s="141"/>
       <c r="U43" s="97"/>
       <c r="V43" s="84"/>
       <c r="W43" s="87"/>
@@ -7647,20 +7637,20 @@
         <v>11.357283333333333</v>
       </c>
       <c r="S44" s="136">
-        <f>R44/H44</f>
+        <f t="shared" ref="S44:S73" si="12">R44/H44</f>
         <v>0.76325828853046584</v>
       </c>
-      <c r="T44" s="150">
-        <f t="shared" si="2"/>
+      <c r="T44" s="140">
+        <f t="shared" si="6"/>
         <v>0.84202037255508067</v>
       </c>
       <c r="U44" s="18"/>
       <c r="V44" s="77">
-        <f>0.001*O44*P44/Z44</f>
+        <f t="shared" ref="V44:V73" si="13">0.001*O44*P44/Z44</f>
         <v>3737.1004416627256</v>
       </c>
       <c r="W44" s="78">
-        <f>Y44*0.01*P44/(O44*0.001)</f>
+        <f t="shared" ref="W44:W73" si="14">Y44*0.01*P44/(O44*0.001)</f>
         <v>1.1299072132232608</v>
       </c>
       <c r="X44" s="3">
@@ -7673,19 +7663,19 @@
         <v>1.5999999999999999E-5</v>
       </c>
       <c r="AA44" s="66">
-        <f t="shared" ref="AA44:AA67" si="5">100*K44/(287*N44)</f>
+        <f t="shared" ref="AA44:AA67" si="15">100*K44/(287*N44)</f>
         <v>119.18565347252668</v>
       </c>
       <c r="AB44" s="67">
-        <f t="shared" ref="AB44:AB67" si="6">SQRT(2000000*Z44/Y44)</f>
+        <f t="shared" ref="AB44:AB67" si="16">SQRT(2000000*Z44/Y44)</f>
         <v>9.1050290721197076</v>
       </c>
       <c r="AC44" s="68">
-        <f>AB44/P44</f>
+        <f t="shared" ref="AC44:AC73" si="17">AB44/P44</f>
         <v>2.1763373830134154</v>
       </c>
-      <c r="AD44" s="153"/>
-      <c r="AE44" s="154"/>
+      <c r="AD44" s="143"/>
+      <c r="AE44" s="144"/>
     </row>
     <row r="45" spans="1:31" ht="15.75">
       <c r="A45" s="43"/>
@@ -7741,20 +7731,20 @@
         <v>13.611287096774193</v>
       </c>
       <c r="S45" s="137">
-        <f>R45/H45</f>
+        <f t="shared" si="12"/>
         <v>0.78951781303794633</v>
       </c>
-      <c r="T45" s="151">
-        <f t="shared" si="2"/>
+      <c r="T45" s="141">
+        <f t="shared" si="6"/>
         <v>0.73578076909567147</v>
       </c>
       <c r="U45" s="32"/>
       <c r="V45" s="79">
-        <f>0.001*O45*P45/Z45</f>
+        <f t="shared" si="13"/>
         <v>4654.8522193554645</v>
       </c>
       <c r="W45" s="80">
-        <f>Y45*0.01*P45/(O45*0.001)</f>
+        <f t="shared" si="14"/>
         <v>1.2997671141473091</v>
       </c>
       <c r="X45" s="7">
@@ -7767,15 +7757,15 @@
         <v>1.5999999999999999E-5</v>
       </c>
       <c r="AA45" s="63">
-        <f t="shared" si="5"/>
+        <f t="shared" si="15"/>
         <v>119.18214164263503</v>
       </c>
       <c r="AB45" s="60">
-        <f t="shared" si="6"/>
+        <f t="shared" si="16"/>
         <v>8.966716793244407</v>
       </c>
       <c r="AC45" s="69">
-        <f>AB45/P45</f>
+        <f t="shared" si="17"/>
         <v>1.8181481848650662</v>
       </c>
     </row>
@@ -7833,20 +7823,20 @@
         <v>15.372322807017541</v>
       </c>
       <c r="S46" s="137">
-        <f>R46/H46</f>
+        <f t="shared" si="12"/>
         <v>0.80567729596528004</v>
       </c>
-      <c r="T46" s="151">
-        <f t="shared" si="2"/>
+      <c r="T46" s="141">
+        <f t="shared" si="6"/>
         <v>0.72978592369539297</v>
       </c>
       <c r="U46" s="32"/>
       <c r="V46" s="79">
-        <f>0.001*O46*P46/Z46</f>
+        <f t="shared" si="13"/>
         <v>3891.0442362418135</v>
       </c>
       <c r="W46" s="80">
-        <f>Y46*0.01*P46/(O46*0.001)</f>
+        <f t="shared" si="14"/>
         <v>1.6500981886021593</v>
       </c>
       <c r="X46" s="7">
@@ -7859,15 +7849,15 @@
         <v>1.5999999999999999E-5</v>
       </c>
       <c r="AA46" s="63">
-        <f t="shared" si="5"/>
+        <f t="shared" si="15"/>
         <v>119.18214164263503</v>
       </c>
       <c r="AB46" s="60">
-        <f t="shared" si="6"/>
+        <f t="shared" si="16"/>
         <v>8.966716793244407</v>
       </c>
       <c r="AC46" s="69">
-        <f>AB46/P46</f>
+        <f t="shared" si="17"/>
         <v>1.7649281091294358</v>
       </c>
     </row>
@@ -7925,20 +7915,20 @@
         <v>16.972218918918919</v>
       </c>
       <c r="S47" s="137">
-        <f>R47/H47</f>
+        <f t="shared" si="12"/>
         <v>0.80133233800372616</v>
       </c>
-      <c r="T47" s="151">
-        <f t="shared" si="2"/>
+      <c r="T47" s="141">
+        <f t="shared" si="6"/>
         <v>0.75423674643742389</v>
       </c>
       <c r="U47" s="32"/>
       <c r="V47" s="79">
-        <f>0.001*O47*P47/Z47</f>
+        <f t="shared" si="13"/>
         <v>5874.1478904469159</v>
       </c>
       <c r="W47" s="80">
-        <f>Y47*0.01*P47/(O47*0.001)</f>
+        <f t="shared" si="14"/>
         <v>1.3179808845497334</v>
       </c>
       <c r="X47" s="7">
@@ -7951,15 +7941,15 @@
         <v>1.5999999999999999E-5</v>
       </c>
       <c r="AA47" s="63">
-        <f t="shared" si="5"/>
+        <f t="shared" si="15"/>
         <v>119.18682408249056</v>
       </c>
       <c r="AB47" s="60">
-        <f t="shared" si="6"/>
+        <f t="shared" si="16"/>
         <v>8.966716793244407</v>
       </c>
       <c r="AC47" s="69">
-        <f>AB47/P47</f>
+        <f t="shared" si="17"/>
         <v>1.6072669110021494</v>
       </c>
     </row>
@@ -8017,20 +8007,20 @@
         <v>18.532246268656717</v>
       </c>
       <c r="S48" s="137">
-        <f>R48/H48</f>
+        <f t="shared" si="12"/>
         <v>0.79742884116423052</v>
       </c>
-      <c r="T48" s="151">
-        <f t="shared" si="2"/>
+      <c r="T48" s="141">
+        <f t="shared" si="6"/>
         <v>0.74477842395536464</v>
       </c>
       <c r="U48" s="32"/>
       <c r="V48" s="79">
-        <f>0.001*O48*P48/Z48</f>
+        <f t="shared" si="13"/>
         <v>5663.6904086348213</v>
       </c>
       <c r="W48" s="80">
-        <f>Y48*0.01*P48/(O48*0.001)</f>
+        <f t="shared" si="14"/>
         <v>1.7548374039587853</v>
       </c>
       <c r="X48" s="7">
@@ -8043,15 +8033,15 @@
         <v>1.5999999999999999E-5</v>
       </c>
       <c r="AA48" s="63">
-        <f t="shared" si="5"/>
+        <f t="shared" si="15"/>
         <v>119.1786298127434</v>
       </c>
       <c r="AB48" s="60">
-        <f t="shared" si="6"/>
+        <f t="shared" si="16"/>
         <v>8.966716793244407</v>
       </c>
       <c r="AC48" s="69">
-        <f>AB48/P48</f>
+        <f t="shared" si="17"/>
         <v>1.418557040667705</v>
       </c>
     </row>
@@ -8109,20 +8099,20 @@
         <v>19.310649999999999</v>
       </c>
       <c r="S49" s="137">
-        <f>R49/H49</f>
+        <f t="shared" si="12"/>
         <v>0.77552811244979925</v>
       </c>
-      <c r="T49" s="151">
-        <f t="shared" si="2"/>
+      <c r="T49" s="141">
+        <f t="shared" si="6"/>
         <v>0.82742270895031922</v>
       </c>
       <c r="U49" s="32"/>
       <c r="V49" s="79">
-        <f>0.001*O49*P49/Z49</f>
+        <f t="shared" si="13"/>
         <v>6163.9402413320668</v>
       </c>
       <c r="W49" s="80">
-        <f>Y49*0.01*P49/(O49*0.001)</f>
+        <f t="shared" si="14"/>
         <v>1.8415029069045974</v>
       </c>
       <c r="X49" s="7">
@@ -8135,15 +8125,15 @@
         <v>1.5999999999999999E-5</v>
       </c>
       <c r="AA49" s="63">
-        <f t="shared" si="5"/>
+        <f t="shared" si="15"/>
         <v>119.17043554299623</v>
       </c>
       <c r="AB49" s="60">
-        <f t="shared" si="6"/>
+        <f t="shared" si="16"/>
         <v>8.966716793244407</v>
       </c>
       <c r="AC49" s="69">
-        <f>AB49/P49</f>
+        <f t="shared" si="17"/>
         <v>1.3273931851568801</v>
       </c>
     </row>
@@ -8201,20 +8191,20 @@
         <v>21.546778947368416</v>
       </c>
       <c r="S50" s="137">
-        <f>R50/H50</f>
+        <f t="shared" si="12"/>
         <v>0.79567130529425467</v>
       </c>
-      <c r="T50" s="151">
-        <f t="shared" si="2"/>
+      <c r="T50" s="141">
+        <f t="shared" si="6"/>
         <v>0.72786519562074081</v>
       </c>
       <c r="U50" s="32"/>
       <c r="V50" s="79">
-        <f>0.001*O50*P50/Z50</f>
+        <f t="shared" si="13"/>
         <v>6954.482338053831</v>
       </c>
       <c r="W50" s="80">
-        <f>Y50*0.01*P50/(O50*0.001)</f>
+        <f t="shared" si="14"/>
         <v>2.0670568248712256</v>
       </c>
       <c r="X50" s="7">
@@ -8227,15 +8217,15 @@
         <v>1.5999999999999999E-5</v>
       </c>
       <c r="AA50" s="63">
-        <f t="shared" si="5"/>
+        <f t="shared" si="15"/>
         <v>119.1540470035019</v>
       </c>
       <c r="AB50" s="60">
-        <f t="shared" si="6"/>
+        <f t="shared" si="16"/>
         <v>8.966716793244407</v>
       </c>
       <c r="AC50" s="69">
-        <f>AB50/P50</f>
+        <f t="shared" si="17"/>
         <v>1.179522923575701</v>
       </c>
     </row>
@@ -8293,20 +8283,20 @@
         <v>23.776596610169495</v>
       </c>
       <c r="S51" s="137">
-        <f>R51/H51</f>
+        <f t="shared" si="12"/>
         <v>0.81454596129391899</v>
       </c>
-      <c r="T51" s="151">
-        <f t="shared" si="2"/>
+      <c r="T51" s="141">
+        <f t="shared" si="6"/>
         <v>0.67253932320086585</v>
       </c>
       <c r="U51" s="32"/>
       <c r="V51" s="79">
-        <f>0.001*O51*P51/Z51</f>
+        <f t="shared" si="13"/>
         <v>6484.6586849485529</v>
       </c>
       <c r="W51" s="80">
-        <f>Y51*0.01*P51/(O51*0.001)</f>
+        <f t="shared" si="14"/>
         <v>2.4853146696383037</v>
       </c>
       <c r="X51" s="7">
@@ -8319,15 +8309,15 @@
         <v>1.5999999999999999E-5</v>
       </c>
       <c r="AA51" s="63">
-        <f t="shared" si="5"/>
+        <f t="shared" si="15"/>
         <v>119.14936456364637</v>
       </c>
       <c r="AB51" s="60">
-        <f t="shared" si="6"/>
+        <f t="shared" si="16"/>
         <v>8.966716793244407</v>
       </c>
       <c r="AC51" s="69">
-        <f>AB51/P51</f>
+        <f t="shared" si="17"/>
         <v>1.1139885963035991</v>
       </c>
     </row>
@@ -8385,20 +8375,20 @@
         <v>25.013867647058824</v>
       </c>
       <c r="S52" s="137">
-        <f>R52/H52</f>
+        <f t="shared" si="12"/>
         <v>0.79967607567323606</v>
       </c>
-      <c r="T52" s="151">
-        <f t="shared" si="2"/>
+      <c r="T52" s="141">
+        <f t="shared" si="6"/>
         <v>0.77556991269276776</v>
       </c>
       <c r="U52" s="32"/>
       <c r="V52" s="79">
-        <f>0.001*O52*P52/Z52</f>
+        <f t="shared" si="13"/>
         <v>6647.6132876863448</v>
       </c>
       <c r="W52" s="80">
-        <f>Y52*0.01*P52/(O52*0.001)</f>
+        <f t="shared" si="14"/>
         <v>2.4119263516121565</v>
       </c>
       <c r="X52" s="7">
@@ -8411,15 +8401,15 @@
         <v>1.5999999999999999E-5</v>
       </c>
       <c r="AA52" s="63">
-        <f t="shared" si="5"/>
+        <f t="shared" si="15"/>
         <v>119.05171274414515</v>
       </c>
       <c r="AB52" s="60">
-        <f t="shared" si="6"/>
+        <f t="shared" si="16"/>
         <v>9.0235766958988304</v>
       </c>
       <c r="AC52" s="69">
-        <f>AB52/P52</f>
+        <f t="shared" si="17"/>
         <v>1.1168635126147399</v>
       </c>
     </row>
@@ -8477,20 +8467,20 @@
         <v>26.412806896551729</v>
       </c>
       <c r="S53" s="138">
-        <f>R53/H53</f>
+        <f t="shared" si="12"/>
         <v>0.79917721320882695</v>
       </c>
-      <c r="T53" s="152">
-        <f t="shared" si="2"/>
+      <c r="T53" s="142">
+        <f t="shared" si="6"/>
         <v>0.79356447718777523</v>
       </c>
       <c r="U53" s="33"/>
       <c r="V53" s="81">
-        <f>0.001*O53*P53/Z53</f>
+        <f t="shared" si="13"/>
         <v>7736.9356263268392</v>
       </c>
       <c r="W53" s="82">
-        <f>Y53*0.01*P53/(O53*0.001)</f>
+        <f t="shared" si="14"/>
         <v>2.2207928617365322</v>
       </c>
       <c r="X53" s="23">
@@ -8503,15 +8493,15 @@
         <v>1.5999999999999999E-5</v>
       </c>
       <c r="AA53" s="72">
-        <f t="shared" si="5"/>
+        <f t="shared" si="15"/>
         <v>119.0552216268818</v>
       </c>
       <c r="AB53" s="73">
-        <f t="shared" si="6"/>
+        <f t="shared" si="16"/>
         <v>9.0235766958988304</v>
       </c>
       <c r="AC53" s="74">
-        <f>AB53/P53</f>
+        <f t="shared" si="17"/>
         <v>1.0788882907933552</v>
       </c>
     </row>
@@ -8569,20 +8559,20 @@
         <v>12.292242857142858</v>
       </c>
       <c r="S54" s="136">
-        <f>R54/H54</f>
+        <f t="shared" si="12"/>
         <v>0.80288980125034992</v>
       </c>
-      <c r="T54" s="150">
-        <f t="shared" si="2"/>
+      <c r="T54" s="140">
+        <f t="shared" si="6"/>
         <v>0.73775197579503671</v>
       </c>
       <c r="U54" s="18"/>
       <c r="V54" s="77">
-        <f>0.001*O54*P54/Z54</f>
+        <f t="shared" si="13"/>
         <v>4793.1254774935296</v>
       </c>
       <c r="W54" s="78">
-        <f>Y54*0.01*P54/(O54*0.001)</f>
+        <f t="shared" si="14"/>
         <v>0.88667145813290404</v>
       </c>
       <c r="X54" s="3">
@@ -8595,19 +8585,19 @@
         <v>1.5E-5</v>
       </c>
       <c r="AA54" s="66">
-        <f t="shared" si="5"/>
+        <f t="shared" si="15"/>
         <v>120.05287366734888</v>
       </c>
       <c r="AB54" s="67">
-        <f t="shared" si="6"/>
+        <f t="shared" si="16"/>
         <v>8.8735650941611386</v>
       </c>
       <c r="AC54" s="68">
-        <f>AB54/P54</f>
+        <f t="shared" si="17"/>
         <v>2.1693230669864922</v>
       </c>
-      <c r="AD54" s="153"/>
-      <c r="AE54" s="154"/>
+      <c r="AD54" s="143"/>
+      <c r="AE54" s="144"/>
     </row>
     <row r="55" spans="1:31" ht="15.75">
       <c r="A55" s="43"/>
@@ -8663,20 +8653,20 @@
         <v>14.476569999999997</v>
       </c>
       <c r="S55" s="137">
-        <f>R55/H55</f>
+        <f t="shared" si="12"/>
         <v>0.8339038018433178</v>
       </c>
-      <c r="T55" s="151">
-        <f t="shared" si="2"/>
+      <c r="T55" s="141">
+        <f t="shared" si="6"/>
         <v>0.62623025125796661</v>
       </c>
       <c r="U55" s="32"/>
       <c r="V55" s="79">
-        <f>0.001*O55*P55/Z55</f>
+        <f t="shared" si="13"/>
         <v>4132.5864915779621</v>
       </c>
       <c r="W55" s="80">
-        <f>Y55*0.01*P55/(O55*0.001)</f>
+        <f t="shared" si="14"/>
         <v>1.3030542700953038</v>
       </c>
       <c r="X55" s="7">
@@ -8689,15 +8679,15 @@
         <v>1.5E-5</v>
       </c>
       <c r="AA55" s="63">
-        <f t="shared" si="5"/>
+        <f t="shared" si="15"/>
         <v>120.0469909718272</v>
       </c>
       <c r="AB55" s="60">
-        <f t="shared" si="6"/>
+        <f t="shared" si="16"/>
         <v>8.8735650941611386</v>
       </c>
       <c r="AC55" s="69">
-        <f>AB55/P55</f>
+        <f t="shared" si="17"/>
         <v>1.9271821748648128</v>
       </c>
     </row>
@@ -8755,20 +8745,20 @@
         <v>15.444204545454546</v>
       </c>
       <c r="S56" s="137">
-        <f>R56/H56</f>
+        <f t="shared" si="12"/>
         <v>0.80944468267581493</v>
       </c>
-      <c r="T56" s="151">
-        <f t="shared" si="2"/>
+      <c r="T56" s="141">
+        <f t="shared" si="6"/>
         <v>0.74444024087234828</v>
       </c>
       <c r="U56" s="32"/>
       <c r="V56" s="79">
-        <f>0.001*O56*P56/Z56</f>
+        <f t="shared" si="13"/>
         <v>5003.6410684306838</v>
       </c>
       <c r="W56" s="80">
-        <f>Y56*0.01*P56/(O56*0.001)</f>
+        <f t="shared" si="14"/>
         <v>1.2457986683211419</v>
       </c>
       <c r="X56" s="7">
@@ -8781,15 +8771,15 @@
         <v>1.5E-5</v>
       </c>
       <c r="AA56" s="63">
-        <f t="shared" si="5"/>
+        <f t="shared" si="15"/>
         <v>120.04816751093153</v>
       </c>
       <c r="AB56" s="60">
-        <f t="shared" si="6"/>
+        <f t="shared" si="16"/>
         <v>8.7481776527970645</v>
       </c>
       <c r="AC56" s="69">
-        <f>AB56/P56</f>
+        <f t="shared" si="17"/>
         <v>1.7912161342576229</v>
       </c>
     </row>
@@ -8847,20 +8837,20 @@
         <v>16.911389285714282</v>
       </c>
       <c r="S57" s="137">
-        <f>R57/H57</f>
+        <f t="shared" si="12"/>
         <v>0.79657980620415836</v>
       </c>
-      <c r="T57" s="151">
-        <f t="shared" si="2"/>
+      <c r="T57" s="141">
+        <f t="shared" si="6"/>
         <v>0.75877680354480981</v>
       </c>
       <c r="U57" s="32"/>
       <c r="V57" s="79">
-        <f>0.001*O57*P57/Z57</f>
+        <f t="shared" si="13"/>
         <v>6136.8787771923562</v>
       </c>
       <c r="W57" s="80">
-        <f>Y57*0.01*P57/(O57*0.001)</f>
+        <f t="shared" si="14"/>
         <v>1.3794542061137296</v>
       </c>
       <c r="X57" s="7">
@@ -8873,15 +8863,15 @@
         <v>1.5E-5</v>
       </c>
       <c r="AA57" s="63">
-        <f t="shared" si="5"/>
+        <f t="shared" si="15"/>
         <v>120.05052058914021</v>
       </c>
       <c r="AB57" s="60">
-        <f t="shared" si="6"/>
+        <f t="shared" si="16"/>
         <v>8.7481776527970645</v>
       </c>
       <c r="AC57" s="69">
-        <f>AB57/P57</f>
+        <f t="shared" si="17"/>
         <v>1.5370485360659276</v>
       </c>
     </row>
@@ -8939,20 +8929,20 @@
         <v>18.811745205479451</v>
       </c>
       <c r="S58" s="137">
-        <f>R58/H58</f>
+        <f t="shared" si="12"/>
         <v>0.80633284206941502</v>
       </c>
-      <c r="T58" s="151">
-        <f t="shared" si="2"/>
+      <c r="T58" s="141">
+        <f t="shared" si="6"/>
         <v>0.74366577929699762</v>
       </c>
       <c r="U58" s="32"/>
       <c r="V58" s="79">
-        <f>0.001*O58*P58/Z58</f>
+        <f t="shared" si="13"/>
         <v>6668.731858458993</v>
       </c>
       <c r="W58" s="80">
-        <f>Y58*0.01*P58/(O58*0.001)</f>
+        <f t="shared" si="14"/>
         <v>1.4465631385691848</v>
       </c>
       <c r="X58" s="7">
@@ -8965,15 +8955,15 @@
         <v>1.5E-5</v>
       </c>
       <c r="AA58" s="63">
-        <f t="shared" si="5"/>
+        <f t="shared" si="15"/>
         <v>120.02816634615782</v>
       </c>
       <c r="AB58" s="60">
-        <f t="shared" si="6"/>
+        <f t="shared" si="16"/>
         <v>8.7481776527970645</v>
       </c>
       <c r="AC58" s="69">
-        <f>AB58/P58</f>
+        <f t="shared" si="17"/>
         <v>1.4398746081087839</v>
       </c>
     </row>
@@ -9031,20 +9021,20 @@
         <v>19.751479999999994</v>
       </c>
       <c r="S59" s="137">
-        <f>R59/H59</f>
+        <f t="shared" si="12"/>
         <v>0.79100841009211031</v>
       </c>
-      <c r="T59" s="151">
-        <f t="shared" si="2"/>
+      <c r="T59" s="141">
+        <f t="shared" si="6"/>
         <v>0.76357267202774415</v>
       </c>
       <c r="U59" s="32"/>
       <c r="V59" s="79">
-        <f>0.001*O59*P59/Z59</f>
+        <f t="shared" si="13"/>
         <v>7324.4938137174167</v>
       </c>
       <c r="W59" s="80">
-        <f>Y59*0.01*P59/(O59*0.001)</f>
+        <f t="shared" si="14"/>
         <v>1.6665223498123918</v>
       </c>
       <c r="X59" s="7">
@@ -9057,15 +9047,15 @@
         <v>1.5E-5</v>
       </c>
       <c r="AA59" s="63">
-        <f t="shared" si="5"/>
+        <f t="shared" si="15"/>
         <v>120.03169596347082</v>
       </c>
       <c r="AB59" s="60">
-        <f t="shared" si="6"/>
+        <f t="shared" si="16"/>
         <v>8.7481776527970645</v>
       </c>
       <c r="AC59" s="69">
-        <f>AB59/P59</f>
+        <f t="shared" si="17"/>
         <v>1.2800313854732082</v>
       </c>
     </row>
@@ -9123,20 +9113,20 @@
         <v>22.048160975609761</v>
       </c>
       <c r="S60" s="137">
-        <f>R60/H60</f>
+        <f t="shared" si="12"/>
         <v>0.81508913033677488</v>
       </c>
-      <c r="T60" s="151">
-        <f t="shared" si="2"/>
+      <c r="T60" s="141">
+        <f t="shared" si="6"/>
         <v>0.66909683973008438</v>
       </c>
       <c r="U60" s="32"/>
       <c r="V60" s="79">
-        <f>0.001*O60*P60/Z60</f>
+        <f t="shared" si="13"/>
         <v>6176.788992136082</v>
       </c>
       <c r="W60" s="80">
-        <f>Y60*0.01*P60/(O60*0.001)</f>
+        <f t="shared" si="14"/>
         <v>2.3862237656799445</v>
       </c>
       <c r="X60" s="7">
@@ -9149,15 +9139,15 @@
         <v>1.5999999999999999E-5</v>
       </c>
       <c r="AA60" s="63">
-        <f t="shared" si="5"/>
+        <f t="shared" si="15"/>
         <v>119.41158119555568</v>
       </c>
       <c r="AB60" s="60">
-        <f t="shared" si="6"/>
+        <f t="shared" si="16"/>
         <v>8.7080068836821631</v>
       </c>
       <c r="AC60" s="69">
-        <f>AB60/P60</f>
+        <f t="shared" si="17"/>
         <v>1.1648715318122116</v>
       </c>
     </row>
@@ -9215,20 +9205,20 @@
         <v>24.000869090909088</v>
       </c>
       <c r="S61" s="137">
-        <f>R61/H61</f>
+        <f t="shared" si="12"/>
         <v>0.82279290678467898</v>
       </c>
-      <c r="T61" s="151">
-        <f t="shared" si="2"/>
+      <c r="T61" s="141">
+        <f t="shared" si="6"/>
         <v>0.69282079634878757</v>
       </c>
       <c r="U61" s="32"/>
       <c r="V61" s="79">
-        <f>0.001*O61*P61/Z61</f>
+        <f t="shared" si="13"/>
         <v>6814.631321267334</v>
       </c>
       <c r="W61" s="80">
-        <f>Y61*0.01*P61/(O61*0.001)</f>
+        <f t="shared" si="14"/>
         <v>2.3178575202931646</v>
       </c>
       <c r="X61" s="7">
@@ -9241,15 +9231,15 @@
         <v>1.5999999999999999E-5</v>
       </c>
       <c r="AA61" s="63">
-        <f t="shared" si="5"/>
+        <f t="shared" si="15"/>
         <v>119.00824325025917</v>
       </c>
       <c r="AB61" s="60">
-        <f t="shared" si="6"/>
+        <f t="shared" si="16"/>
         <v>8.3955096032222691</v>
       </c>
       <c r="AC61" s="69">
-        <f>AB61/P61</f>
+        <f t="shared" si="17"/>
         <v>1.1252536937744722</v>
       </c>
     </row>
@@ -9307,20 +9297,20 @@
         <v>25.148703703703703</v>
       </c>
       <c r="S62" s="137">
-        <f>R62/H62</f>
+        <f t="shared" si="12"/>
         <v>0.81387390626872824</v>
       </c>
-      <c r="T62" s="151">
-        <f t="shared" si="2"/>
+      <c r="T62" s="141">
+        <f t="shared" si="6"/>
         <v>0.74305041518384995</v>
       </c>
       <c r="U62" s="32"/>
       <c r="V62" s="79">
-        <f>0.001*O62*P62/Z62</f>
+        <f t="shared" si="13"/>
         <v>7946.3013132179885</v>
       </c>
       <c r="W62" s="80">
-        <f>Y62*0.01*P62/(O62*0.001)</f>
+        <f t="shared" si="14"/>
         <v>2.1160246860821932</v>
       </c>
       <c r="X62" s="7">
@@ -9333,15 +9323,15 @@
         <v>1.5E-5</v>
       </c>
       <c r="AA62" s="63">
-        <f t="shared" si="5"/>
+        <f t="shared" si="15"/>
         <v>119.62071737253035</v>
       </c>
       <c r="AB62" s="60">
-        <f t="shared" si="6"/>
+        <f t="shared" si="16"/>
         <v>8.4414991182502899</v>
       </c>
       <c r="AC62" s="69">
-        <f>AB62/P62</f>
+        <f t="shared" si="17"/>
         <v>1.0906166369187591</v>
       </c>
     </row>
@@ -9399,20 +9389,20 @@
         <v>26.647783018867933</v>
       </c>
       <c r="S63" s="138">
-        <f>R63/H63</f>
+        <f t="shared" si="12"/>
         <v>0.80653096304079708</v>
       </c>
-      <c r="T63" s="152">
-        <f t="shared" si="2"/>
+      <c r="T63" s="142">
+        <f t="shared" si="6"/>
         <v>0.73319609707281641</v>
       </c>
       <c r="U63" s="33"/>
       <c r="V63" s="81">
-        <f>0.001*O63*P63/Z63</f>
+        <f t="shared" si="13"/>
         <v>10393.389230157703</v>
       </c>
       <c r="W63" s="82">
-        <f>Y63*0.01*P63/(O63*0.001)</f>
+        <f t="shared" si="14"/>
         <v>2.0525624190057266</v>
       </c>
       <c r="X63" s="23">
@@ -9425,15 +9415,15 @@
         <v>1.5E-5</v>
       </c>
       <c r="AA63" s="72">
-        <f t="shared" si="5"/>
+        <f t="shared" si="15"/>
         <v>119.61368189437286</v>
       </c>
       <c r="AB63" s="73">
-        <f t="shared" si="6"/>
+        <f t="shared" si="16"/>
         <v>8.4414991182502899</v>
       </c>
       <c r="AC63" s="74">
-        <f>AB63/P63</f>
+        <f t="shared" si="17"/>
         <v>0.96825158238740039</v>
       </c>
     </row>
@@ -9491,20 +9481,20 @@
         <v>12.88167777777778</v>
       </c>
       <c r="S64" s="136">
-        <f>R64/H64</f>
+        <f t="shared" si="12"/>
         <v>0.84138979606647812</v>
       </c>
-      <c r="T64" s="150">
-        <f t="shared" si="2"/>
+      <c r="T64" s="140">
+        <f t="shared" si="6"/>
         <v>0.57158410830435058</v>
       </c>
       <c r="U64" s="18"/>
       <c r="V64" s="77">
-        <f>0.001*O64*P64/Z64</f>
+        <f t="shared" si="13"/>
         <v>4352.0846396056122</v>
       </c>
       <c r="W64" s="78">
-        <f>Y64*0.01*P64/(O64*0.001)</f>
+        <f t="shared" si="14"/>
         <v>1.1999232672598319</v>
       </c>
       <c r="X64" s="3">
@@ -9517,19 +9507,19 @@
         <v>1.5E-5</v>
       </c>
       <c r="AA64" s="66">
-        <f t="shared" si="5"/>
+        <f t="shared" si="15"/>
         <v>119.57615934419965</v>
       </c>
       <c r="AB64" s="67">
-        <f t="shared" si="6"/>
+        <f t="shared" si="16"/>
         <v>8.3141099321053993</v>
       </c>
       <c r="AC64" s="68">
-        <f>AB64/P64</f>
+        <f t="shared" si="17"/>
         <v>1.9569944500767018</v>
       </c>
-      <c r="AD64" s="153"/>
-      <c r="AE64" s="154"/>
+      <c r="AD64" s="143"/>
+      <c r="AE64" s="144"/>
     </row>
     <row r="65" spans="1:29" ht="15.75">
       <c r="A65" s="43"/>
@@ -9585,20 +9575,20 @@
         <v>14.180497777777783</v>
       </c>
       <c r="S65" s="137">
-        <f>R65/H65</f>
+        <f t="shared" si="12"/>
         <v>0.83512943332024625</v>
       </c>
-      <c r="T65" s="151">
-        <f t="shared" si="2"/>
+      <c r="T65" s="141">
+        <f t="shared" si="6"/>
         <v>0.62951469589537612</v>
       </c>
       <c r="U65" s="32"/>
       <c r="V65" s="79">
-        <f>0.001*O65*P65/Z65</f>
+        <f t="shared" si="13"/>
         <v>4464.9150160867448</v>
       </c>
       <c r="W65" s="80">
-        <f>Y65*0.01*P65/(O65*0.001)</f>
+        <f t="shared" si="14"/>
         <v>1.2815488356127303</v>
       </c>
       <c r="X65" s="7">
@@ -9611,15 +9601,15 @@
         <v>1.5E-5</v>
       </c>
       <c r="AA65" s="63">
-        <f t="shared" si="5"/>
+        <f t="shared" si="15"/>
         <v>119.56677870665634</v>
       </c>
       <c r="AB65" s="60">
-        <f t="shared" si="6"/>
+        <f t="shared" si="16"/>
         <v>8.3141099321053993</v>
       </c>
       <c r="AC65" s="69">
-        <f>AB65/P65</f>
+        <f t="shared" si="17"/>
         <v>1.8695660764274991</v>
       </c>
     </row>
@@ -9677,20 +9667,20 @@
         <v>15.155106666666658</v>
       </c>
       <c r="S66" s="137">
-        <f>R66/H66</f>
+        <f t="shared" si="12"/>
         <v>0.79346108202443233</v>
       </c>
-      <c r="T66" s="151">
-        <f t="shared" si="2"/>
+      <c r="T66" s="141">
+        <f t="shared" si="6"/>
         <v>0.80699009816234024</v>
       </c>
       <c r="U66" s="32"/>
       <c r="V66" s="79">
-        <f>0.001*O66*P66/Z66</f>
+        <f t="shared" si="13"/>
         <v>5695.9346035477602</v>
       </c>
       <c r="W66" s="80">
-        <f>Y66*0.01*P66/(O66*0.001)</f>
+        <f t="shared" si="14"/>
         <v>1.2138571859954321</v>
       </c>
       <c r="X66" s="7">
@@ -9703,15 +9693,15 @@
         <v>1.5E-5</v>
       </c>
       <c r="AA66" s="63">
-        <f t="shared" si="5"/>
+        <f t="shared" si="15"/>
         <v>119.55739806911303</v>
       </c>
       <c r="AB66" s="60">
-        <f t="shared" si="6"/>
+        <f t="shared" si="16"/>
         <v>8.3141099321053993</v>
       </c>
       <c r="AC66" s="69">
-        <f>AB66/P66</f>
+        <f t="shared" si="17"/>
         <v>1.7007822071003711</v>
       </c>
     </row>
@@ -9769,20 +9759,20 @@
         <v>17.196181250000002</v>
       </c>
       <c r="S67" s="137">
-        <f>R67/H67</f>
+        <f t="shared" si="12"/>
         <v>0.81305821513002385</v>
       </c>
-      <c r="T67" s="151">
-        <f t="shared" si="2"/>
+      <c r="T67" s="141">
+        <f t="shared" si="6"/>
         <v>0.69968861682067307</v>
       </c>
       <c r="U67" s="32"/>
       <c r="V67" s="79">
-        <f>0.001*O67*P67/Z67</f>
+        <f t="shared" si="13"/>
         <v>5240.4148651176538</v>
       </c>
       <c r="W67" s="80">
-        <f>Y67*0.01*P67/(O67*0.001)</f>
+        <f t="shared" si="14"/>
         <v>1.7137629814200896</v>
       </c>
       <c r="X67" s="7">
@@ -9795,20 +9785,20 @@
         <v>1.5999999999999999E-5</v>
       </c>
       <c r="AA67" s="63">
-        <f t="shared" si="5"/>
+        <f t="shared" si="15"/>
         <v>119.3436858176506</v>
       </c>
       <c r="AB67" s="60">
-        <f t="shared" si="6"/>
+        <f t="shared" si="16"/>
         <v>8.4327404271156787</v>
       </c>
       <c r="AC67" s="69">
-        <f>AB67/P67</f>
+        <f t="shared" si="17"/>
         <v>1.4923022168015028</v>
       </c>
     </row>
     <row r="68" spans="1:29" ht="15.75">
-      <c r="A68" s="142"/>
+      <c r="A68" s="148"/>
       <c r="B68" s="6">
         <v>65</v>
       </c>
@@ -9819,7 +9809,7 @@
         <v>23</v>
       </c>
       <c r="E68" s="7">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="F68" s="7">
         <v>65</v>
@@ -9861,20 +9851,20 @@
         <v>19.037488888888888</v>
       </c>
       <c r="S68" s="137">
-        <f>R68/H68</f>
+        <f t="shared" si="12"/>
         <v>0.81952169129956465</v>
       </c>
-      <c r="T68" s="151">
-        <f t="shared" si="2"/>
+      <c r="T68" s="141">
+        <f t="shared" si="6"/>
         <v>0.65119907017359535</v>
       </c>
       <c r="U68" s="32"/>
       <c r="V68" s="79">
-        <f>0.001*O68*P68/Z68</f>
+        <f t="shared" si="13"/>
         <v>7001.0805318948824</v>
       </c>
       <c r="W68" s="80">
-        <f>Y68*0.01*P68/(O68*0.001)</f>
+        <f t="shared" si="14"/>
         <v>1.5615226785174976</v>
       </c>
       <c r="X68" s="7">
@@ -9887,20 +9877,20 @@
         <v>1.5999999999999999E-5</v>
       </c>
       <c r="AA68" s="63">
-        <f t="shared" ref="AA68:AA73" si="7">100*K68/(287*N68)</f>
+        <f t="shared" ref="AA68:AA73" si="18">100*K68/(287*N68)</f>
         <v>119.34719764754223</v>
       </c>
       <c r="AB68" s="60">
-        <f t="shared" ref="AB68:AB73" si="8">SQRT(2000000*Z68/Y68)</f>
+        <f t="shared" ref="AB68:AB73" si="19">SQRT(2000000*Z68/Y68)</f>
         <v>8.7080068836821631</v>
       </c>
       <c r="AC68" s="69">
-        <f>AB68/P68</f>
+        <f t="shared" si="17"/>
         <v>1.3525655234855751</v>
       </c>
     </row>
     <row r="69" spans="1:29" ht="15.75">
-      <c r="A69" s="142"/>
+      <c r="A69" s="148"/>
       <c r="B69" s="6">
         <v>66</v>
       </c>
@@ -9953,20 +9943,20 @@
         <v>20.399920000000002</v>
       </c>
       <c r="S69" s="137">
-        <f>R69/H69</f>
+        <f t="shared" si="12"/>
         <v>0.81730448717948723</v>
       </c>
-      <c r="T69" s="151">
-        <f t="shared" ref="T69:T73" si="9">(H69-R69)/P69</f>
+      <c r="T69" s="141">
+        <f t="shared" ref="T69:T73" si="20">(H69-R69)/P69</f>
         <v>0.64911459110621561</v>
       </c>
       <c r="U69" s="32"/>
       <c r="V69" s="79">
-        <f>0.001*O69*P69/Z69</f>
+        <f t="shared" si="13"/>
         <v>6791.5692457114274</v>
       </c>
       <c r="W69" s="80">
-        <f>Y69*0.01*P69/(O69*0.001)</f>
+        <f t="shared" si="14"/>
         <v>1.9165692495655877</v>
       </c>
       <c r="X69" s="7">
@@ -9979,20 +9969,20 @@
         <v>1.5999999999999999E-5</v>
       </c>
       <c r="AA69" s="63">
-        <f t="shared" si="7"/>
+        <f t="shared" si="18"/>
         <v>119.34485642761447</v>
       </c>
       <c r="AB69" s="60">
-        <f t="shared" si="8"/>
+        <f t="shared" si="19"/>
         <v>8.7080068836821631</v>
       </c>
       <c r="AC69" s="69">
-        <f>AB69/P69</f>
+        <f t="shared" si="17"/>
         <v>1.2395603427245705</v>
       </c>
     </row>
     <row r="70" spans="1:29" ht="15.75">
-      <c r="A70" s="142"/>
+      <c r="A70" s="148"/>
       <c r="B70" s="6">
         <v>67</v>
       </c>
@@ -10045,20 +10035,20 @@
         <v>22.16266818181818</v>
       </c>
       <c r="S70" s="137">
-        <f>R70/H70</f>
+        <f t="shared" si="12"/>
         <v>0.81932229877331531</v>
       </c>
-      <c r="T70" s="151">
-        <f t="shared" si="9"/>
+      <c r="T70" s="141">
+        <f t="shared" si="20"/>
         <v>0.6770406927512661</v>
       </c>
       <c r="U70" s="32"/>
       <c r="V70" s="79">
-        <f>0.001*O70*P70/Z70</f>
+        <f t="shared" si="13"/>
         <v>6060.1478700079506</v>
       </c>
       <c r="W70" s="80">
-        <f>Y70*0.01*P70/(O70*0.001)</f>
+        <f t="shared" si="14"/>
         <v>2.2678971445229115</v>
       </c>
       <c r="X70" s="7">
@@ -10071,20 +10061,20 @@
         <v>1.5999999999999999E-5</v>
       </c>
       <c r="AA70" s="63">
-        <f t="shared" si="7"/>
+        <f t="shared" si="18"/>
         <v>119.32729727815627</v>
       </c>
       <c r="AB70" s="60">
-        <f t="shared" si="8"/>
+        <f t="shared" si="19"/>
         <v>8.7080068836821631</v>
       </c>
       <c r="AC70" s="69">
-        <f>AB70/P70</f>
+        <f t="shared" si="17"/>
         <v>1.2063177276152834</v>
       </c>
     </row>
     <row r="71" spans="1:29" ht="15.75">
-      <c r="A71" s="142"/>
+      <c r="A71" s="148"/>
       <c r="B71" s="6">
         <v>68</v>
       </c>
@@ -10137,20 +10127,20 @@
         <v>23.687436111111115</v>
       </c>
       <c r="S71" s="137">
-        <f>R71/H71</f>
+        <f t="shared" si="12"/>
         <v>0.81204786119681571</v>
       </c>
-      <c r="T71" s="151">
-        <f t="shared" si="9"/>
+      <c r="T71" s="141">
+        <f t="shared" si="20"/>
         <v>0.73730277630278307</v>
       </c>
       <c r="U71" s="32"/>
       <c r="V71" s="79">
-        <f>0.001*O71*P71/Z71</f>
+        <f t="shared" si="13"/>
         <v>6946.0624586928934</v>
       </c>
       <c r="W71" s="80">
-        <f>Y71*0.01*P71/(O71*0.001)</f>
+        <f t="shared" si="14"/>
         <v>2.0995655984315458</v>
       </c>
       <c r="X71" s="7">
@@ -10163,20 +10153,20 @@
         <v>1.5999999999999999E-5</v>
       </c>
       <c r="AA71" s="63">
-        <f t="shared" si="7"/>
+        <f t="shared" si="18"/>
         <v>119.31793239844521</v>
       </c>
       <c r="AB71" s="60">
-        <f t="shared" si="8"/>
+        <f t="shared" si="19"/>
         <v>8.7080068836821631</v>
       </c>
       <c r="AC71" s="69">
-        <f>AB71/P71</f>
+        <f t="shared" si="17"/>
         <v>1.1710648122887248</v>
       </c>
     </row>
     <row r="72" spans="1:29" ht="15.75">
-      <c r="A72" s="142"/>
+      <c r="A72" s="148"/>
       <c r="B72" s="6">
         <v>69</v>
       </c>
@@ -10229,20 +10219,20 @@
         <v>25.637371428571431</v>
       </c>
       <c r="S72" s="137">
-        <f>R72/H72</f>
+        <f t="shared" si="12"/>
         <v>0.81882374412556469</v>
       </c>
-      <c r="T72" s="151">
-        <f t="shared" si="9"/>
+      <c r="T72" s="141">
+        <f t="shared" si="20"/>
         <v>0.70191711392224121</v>
       </c>
       <c r="U72" s="32"/>
       <c r="V72" s="79">
-        <f>0.001*O72*P72/Z72</f>
+        <f t="shared" si="13"/>
         <v>9724.590397897251</v>
       </c>
       <c r="W72" s="80">
-        <f>Y72*0.01*P72/(O72*0.001)</f>
+        <f t="shared" si="14"/>
         <v>1.7714062957584398</v>
       </c>
       <c r="X72" s="7">
@@ -10255,20 +10245,20 @@
         <v>1.5999999999999999E-5</v>
       </c>
       <c r="AA72" s="63">
-        <f t="shared" si="7"/>
+        <f t="shared" si="18"/>
         <v>119.30973812869804</v>
       </c>
       <c r="AB72" s="60">
-        <f t="shared" si="8"/>
+        <f t="shared" si="19"/>
         <v>8.7080068836821631</v>
       </c>
       <c r="AC72" s="69">
-        <f>AB72/P72</f>
+        <f t="shared" si="17"/>
         <v>1.0775073641512725</v>
       </c>
     </row>
     <row r="73" spans="1:29" ht="16.5" thickBot="1">
-      <c r="A73" s="143"/>
+      <c r="A73" s="149"/>
       <c r="B73" s="15">
         <v>70</v>
       </c>
@@ -10321,20 +10311,20 @@
         <v>27.145739024390238</v>
       </c>
       <c r="S73" s="138">
-        <f>R73/H73</f>
+        <f t="shared" si="12"/>
         <v>0.82234895560103727</v>
       </c>
-      <c r="T73" s="152">
-        <f t="shared" si="9"/>
+      <c r="T73" s="142">
+        <f t="shared" si="20"/>
         <v>0.66905868188398088</v>
       </c>
       <c r="U73" s="33"/>
       <c r="V73" s="81">
-        <f>0.001*O73*P73/Z73</f>
+        <f t="shared" si="13"/>
         <v>8395.1517526041716</v>
       </c>
       <c r="W73" s="82">
-        <f>Y73*0.01*P73/(O73*0.001)</f>
+        <f t="shared" si="14"/>
         <v>2.4135820921156816</v>
       </c>
       <c r="X73" s="23">
@@ -10347,15 +10337,15 @@
         <v>1.5999999999999999E-5</v>
       </c>
       <c r="AA73" s="72">
-        <f t="shared" si="7"/>
+        <f t="shared" si="18"/>
         <v>119.31090873866192</v>
       </c>
       <c r="AB73" s="73">
-        <f t="shared" si="8"/>
+        <f t="shared" si="19"/>
         <v>8.7080068836821631</v>
       </c>
       <c r="AC73" s="74">
-        <f>AB73/P73</f>
+        <f t="shared" si="17"/>
         <v>0.99350414854741709</v>
       </c>
     </row>
@@ -10402,12 +10392,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:22" ht="15.75" thickBot="1">
-      <c r="H1" s="141"/>
-      <c r="I1" s="141"/>
-      <c r="M1" s="140" t="s">
+      <c r="H1" s="147"/>
+      <c r="I1" s="147"/>
+      <c r="M1" s="146" t="s">
         <v>30</v>
       </c>
-      <c r="N1" s="140"/>
+      <c r="N1" s="146"/>
       <c r="O1" s="47"/>
     </row>
     <row r="2" spans="2:22" ht="15.75" thickBot="1">
@@ -10453,15 +10443,15 @@
       <c r="O2" s="40" t="s">
         <v>33</v>
       </c>
-      <c r="P2" s="146" t="s">
+      <c r="P2" s="152" t="s">
         <v>57</v>
       </c>
-      <c r="Q2" s="147"/>
-      <c r="R2" s="147"/>
-      <c r="S2" s="147"/>
-      <c r="T2" s="147"/>
-      <c r="U2" s="147"/>
-      <c r="V2" s="148"/>
+      <c r="Q2" s="153"/>
+      <c r="R2" s="153"/>
+      <c r="S2" s="153"/>
+      <c r="T2" s="153"/>
+      <c r="U2" s="153"/>
+      <c r="V2" s="154"/>
     </row>
     <row r="3" spans="2:22" ht="15.75" thickBot="1">
       <c r="B3" s="10" t="s">

</xml_diff>